<commit_message>
Documentatie: Planning + Taakverdeling + Rolverdeling.xlsx geupdate.
</commit_message>
<xml_diff>
--- a/Documentatie/Planning + Taakverdeling + Rolverdeling/Planning + Taakverdeling + Rolverdeling.xlsx
+++ b/Documentatie/Planning + Taakverdeling + Rolverdeling/Planning + Taakverdeling + Rolverdeling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Onderdeel:</t>
   </si>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t>&gt;&gt; Opdrachtbeschrijving, globale (ruwe) taakverdeling en planning en mijlpalen, Eisen / wensen overzicht (tabel 'versimpelen'?)</t>
+  </si>
+  <si>
+    <t>xmlParser</t>
+  </si>
+  <si>
+    <t>networkConnection</t>
+  </si>
+  <si>
+    <t>Remco en Yme</t>
+  </si>
+  <si>
+    <t>Remco</t>
   </si>
 </sst>
 </file>
@@ -586,7 +598,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -648,6 +660,24 @@
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="1" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,6 +686,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -671,51 +725,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1036,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z90"/>
+  <dimension ref="A1:Z96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,14 +1061,14 @@
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1070,23 +1079,23 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="55" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="55"/>
+      <c r="G4" s="50"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="2"/>
       <c r="F5" s="16">
         <v>46</v>
@@ -1120,12 +1129,12 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="2"/>
       <c r="F6" s="35"/>
       <c r="G6" s="2"/>
@@ -1133,20 +1142,20 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="50" t="s">
+      <c r="L6" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="50"/>
+      <c r="M6" s="53"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="2"/>
       <c r="F7" s="26"/>
       <c r="G7" s="35"/>
@@ -1154,18 +1163,18 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="39"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="2"/>
       <c r="F8" s="26"/>
       <c r="G8" s="2"/>
@@ -1173,18 +1182,18 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="2"/>
       <c r="F9" s="26"/>
       <c r="G9" s="2"/>
@@ -1192,18 +1201,18 @@
       <c r="I9" s="35"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="2"/>
       <c r="F10" s="26"/>
       <c r="G10" s="2"/>
@@ -1211,18 +1220,18 @@
       <c r="I10" s="35"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="2"/>
       <c r="F11" s="26"/>
       <c r="G11" s="2"/>
@@ -1230,18 +1239,18 @@
       <c r="I11" s="2"/>
       <c r="J11" s="35"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="2"/>
       <c r="F12" s="26"/>
       <c r="G12" s="2"/>
@@ -1249,18 +1258,18 @@
       <c r="I12" s="2"/>
       <c r="J12" s="35"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="2"/>
       <c r="F13" s="26"/>
       <c r="G13" s="2"/>
@@ -1268,18 +1277,18 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="35"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="2"/>
       <c r="F14" s="26"/>
       <c r="G14" s="2"/>
@@ -1287,18 +1296,18 @@
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="35"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1306,18 +1315,18 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
       <c r="N15" s="9"/>
       <c r="O15" s="35"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="2"/>
       <c r="F16" s="26"/>
       <c r="G16" s="2"/>
@@ -1325,16 +1334,16 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
       <c r="N16" s="3"/>
       <c r="O16" s="35"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="2"/>
       <c r="F17" s="26"/>
       <c r="G17" s="2"/>
@@ -1342,16 +1351,16 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
       <c r="E18" s="2"/>
       <c r="F18" s="26"/>
       <c r="G18" s="2"/>
@@ -1359,18 +1368,18 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="3"/>
@@ -1378,453 +1387,452 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
       <c r="N19" s="9"/>
       <c r="O19" s="35"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="32"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
       <c r="N20" s="32"/>
       <c r="O20" s="32"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="52"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="36"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="39"/>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="28"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="36"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="45"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="36"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
       <c r="N26" s="33"/>
       <c r="O26" s="33"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="31"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="27"/>
       <c r="O27" s="28"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="36"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="46"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="35"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="28"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="49"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="35"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
       <c r="H30" s="26"/>
       <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
       <c r="N30" s="31"/>
       <c r="O30" s="28"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="28"/>
-      <c r="Q31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="26"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="2"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="26"/>
       <c r="I32" s="26"/>
       <c r="J32" s="26"/>
       <c r="K32" s="26"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="27"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="31"/>
       <c r="O32" s="28"/>
-      <c r="Q32" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="57"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
+      <c r="A33" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="35"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
       <c r="J33" s="26"/>
       <c r="K33" s="26"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="27"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="31"/>
       <c r="O33" s="28"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A34" s="57"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="59"/>
+      <c r="A34" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
       <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="35"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
       <c r="J34" s="26"/>
       <c r="K34" s="26"/>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
       <c r="N34" s="27"/>
       <c r="O34" s="28"/>
+      <c r="Q34" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A35" s="57"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
+      <c r="A35" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
       <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="35"/>
       <c r="I35" s="26"/>
       <c r="J35" s="26"/>
       <c r="K35" s="26"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
       <c r="N35" s="27"/>
       <c r="O35" s="28"/>
+      <c r="Q35" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="28"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="40"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="28"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="40"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="28"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="28"/>
-      <c r="Q36" t="s">
+      <c r="B39" s="41"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="28"/>
+      <c r="Q39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="28"/>
-      <c r="Q37" t="s">
+      <c r="B40" s="41"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="53"/>
+      <c r="M40" s="53"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="28"/>
+      <c r="Q40" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B40" s="5"/>
-      <c r="C40" s="53" t="s">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="53"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="53" t="s">
+      <c r="D43" s="48"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="53"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="53" t="s">
+      <c r="G43" s="48"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="J40" s="53"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="53" t="s">
+      <c r="J43" s="48"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A46" s="51" t="s">
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B49" s="47" t="s">
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B52" s="37" t="s">
         <v>9</v>
-      </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="49"/>
-      <c r="J49" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="49"/>
-    </row>
-    <row r="50" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B50" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="39"/>
-      <c r="J50" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="39"/>
-    </row>
-    <row r="51" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B51" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="39"/>
-      <c r="J51" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
-      <c r="M51" s="38"/>
-      <c r="N51" s="38"/>
-      <c r="O51" s="39"/>
-      <c r="W51" s="13"/>
-      <c r="X51" s="13"/>
-      <c r="Y51" s="13"/>
-      <c r="Z51" s="13"/>
-    </row>
-    <row r="52" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B52" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="C52" s="38"/>
       <c r="D52" s="38"/>
@@ -1832,367 +1840,371 @@
       <c r="F52" s="38"/>
       <c r="G52" s="39"/>
       <c r="J52" s="37" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="K52" s="38"/>
       <c r="L52" s="38"/>
       <c r="M52" s="38"/>
       <c r="N52" s="38"/>
       <c r="O52" s="39"/>
-      <c r="W52" s="14"/>
-      <c r="X52" s="14"/>
-      <c r="Y52" s="14"/>
-      <c r="Z52" s="14"/>
-    </row>
-    <row r="53" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B53" s="37" t="s">
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B53" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+      <c r="J53" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K53" s="44"/>
+      <c r="L53" s="44"/>
+      <c r="M53" s="44"/>
+      <c r="N53" s="44"/>
+      <c r="O53" s="45"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B54" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="45"/>
+      <c r="J54" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K54" s="44"/>
+      <c r="L54" s="44"/>
+      <c r="M54" s="44"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="45"/>
+      <c r="W54" s="13"/>
+      <c r="X54" s="13"/>
+      <c r="Y54" s="13"/>
+      <c r="Z54" s="13"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B55" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="39"/>
-      <c r="J53" s="37" t="s">
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="45"/>
+      <c r="J55" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38"/>
-      <c r="M53" s="38"/>
-      <c r="N53" s="38"/>
-      <c r="O53" s="39"/>
-      <c r="W53" s="14"/>
-      <c r="X53" s="14"/>
-      <c r="Y53" s="14"/>
-      <c r="Z53" s="14"/>
-    </row>
-    <row r="54" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B54" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="39"/>
-      <c r="J54" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="K54" s="38"/>
-      <c r="L54" s="38"/>
-      <c r="M54" s="38"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="39"/>
-      <c r="W54" s="14"/>
-      <c r="X54" s="14"/>
-      <c r="Y54" s="14"/>
-      <c r="Z54" s="14"/>
-    </row>
-    <row r="55" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B55" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="39"/>
-      <c r="J55" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="K55" s="38"/>
-      <c r="L55" s="38"/>
-      <c r="M55" s="38"/>
-      <c r="N55" s="38"/>
-      <c r="O55" s="39"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="44"/>
+      <c r="M55" s="44"/>
+      <c r="N55" s="44"/>
+      <c r="O55" s="45"/>
       <c r="W55" s="14"/>
       <c r="X55" s="14"/>
       <c r="Y55" s="14"/>
       <c r="Z55" s="14"/>
     </row>
-    <row r="56" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B56" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="39"/>
-      <c r="J56" s="37" t="s">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B56" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
+      <c r="J56" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K56" s="38"/>
-      <c r="L56" s="38"/>
-      <c r="M56" s="38"/>
-      <c r="N56" s="38"/>
-      <c r="O56" s="39"/>
+      <c r="K56" s="44"/>
+      <c r="L56" s="44"/>
+      <c r="M56" s="44"/>
+      <c r="N56" s="44"/>
+      <c r="O56" s="45"/>
       <c r="W56" s="14"/>
       <c r="X56" s="14"/>
       <c r="Y56" s="14"/>
       <c r="Z56" s="14"/>
     </row>
-    <row r="57" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B57" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="39"/>
-      <c r="J57" s="37" t="s">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B57" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="45"/>
+      <c r="J57" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K57" s="38"/>
-      <c r="L57" s="38"/>
-      <c r="M57" s="38"/>
-      <c r="N57" s="38"/>
-      <c r="O57" s="39"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="44"/>
+      <c r="M57" s="44"/>
+      <c r="N57" s="44"/>
+      <c r="O57" s="45"/>
       <c r="W57" s="14"/>
       <c r="X57" s="14"/>
       <c r="Y57" s="14"/>
       <c r="Z57" s="14"/>
     </row>
-    <row r="58" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B58" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="39"/>
-      <c r="J58" s="37" t="s">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B58" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="45"/>
+      <c r="J58" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K58" s="38"/>
-      <c r="L58" s="38"/>
-      <c r="M58" s="38"/>
-      <c r="N58" s="38"/>
-      <c r="O58" s="39"/>
+      <c r="K58" s="44"/>
+      <c r="L58" s="44"/>
+      <c r="M58" s="44"/>
+      <c r="N58" s="44"/>
+      <c r="O58" s="45"/>
       <c r="W58" s="14"/>
       <c r="X58" s="14"/>
       <c r="Y58" s="14"/>
       <c r="Z58" s="14"/>
     </row>
-    <row r="59" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B59" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="39"/>
-      <c r="J59" s="37" t="s">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B59" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="45"/>
+      <c r="J59" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K59" s="38"/>
-      <c r="L59" s="38"/>
-      <c r="M59" s="38"/>
-      <c r="N59" s="38"/>
-      <c r="O59" s="39"/>
+      <c r="K59" s="44"/>
+      <c r="L59" s="44"/>
+      <c r="M59" s="44"/>
+      <c r="N59" s="44"/>
+      <c r="O59" s="45"/>
       <c r="W59" s="14"/>
       <c r="X59" s="14"/>
       <c r="Y59" s="14"/>
       <c r="Z59" s="14"/>
     </row>
-    <row r="60" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B60" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="38"/>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="39"/>
-      <c r="J60" s="37" t="s">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B60" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="45"/>
+      <c r="J60" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K60" s="38"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="38"/>
-      <c r="O60" s="39"/>
+      <c r="K60" s="44"/>
+      <c r="L60" s="44"/>
+      <c r="M60" s="44"/>
+      <c r="N60" s="44"/>
+      <c r="O60" s="45"/>
       <c r="W60" s="14"/>
       <c r="X60" s="14"/>
       <c r="Y60" s="14"/>
       <c r="Z60" s="14"/>
     </row>
-    <row r="61" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B61" s="37"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="39"/>
-      <c r="J61" s="37"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="38"/>
-      <c r="M61" s="38"/>
-      <c r="N61" s="38"/>
-      <c r="O61" s="39"/>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B61" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="45"/>
+      <c r="J61" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="44"/>
+      <c r="L61" s="44"/>
+      <c r="M61" s="44"/>
+      <c r="N61" s="44"/>
+      <c r="O61" s="45"/>
       <c r="W61" s="14"/>
       <c r="X61" s="14"/>
       <c r="Y61" s="14"/>
       <c r="Z61" s="14"/>
     </row>
-    <row r="62" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="39"/>
-      <c r="J62" s="37"/>
-      <c r="K62" s="38"/>
-      <c r="L62" s="38"/>
-      <c r="M62" s="38"/>
-      <c r="N62" s="38"/>
-      <c r="O62" s="39"/>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B62" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="45"/>
+      <c r="J62" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K62" s="44"/>
+      <c r="L62" s="44"/>
+      <c r="M62" s="44"/>
+      <c r="N62" s="44"/>
+      <c r="O62" s="45"/>
       <c r="W62" s="14"/>
       <c r="X62" s="14"/>
       <c r="Y62" s="14"/>
       <c r="Z62" s="14"/>
     </row>
-    <row r="63" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B63" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
-      <c r="F63" s="41"/>
-      <c r="G63" s="42"/>
-      <c r="J63" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="K63" s="38"/>
-      <c r="L63" s="38"/>
-      <c r="M63" s="38"/>
-      <c r="N63" s="38"/>
-      <c r="O63" s="39"/>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B63" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="45"/>
+      <c r="J63" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K63" s="44"/>
+      <c r="L63" s="44"/>
+      <c r="M63" s="44"/>
+      <c r="N63" s="44"/>
+      <c r="O63" s="45"/>
       <c r="W63" s="14"/>
       <c r="X63" s="14"/>
       <c r="Y63" s="14"/>
       <c r="Z63" s="14"/>
     </row>
-    <row r="64" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B64" s="47"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="49"/>
-      <c r="J64" s="37"/>
-      <c r="K64" s="38"/>
-      <c r="L64" s="38"/>
-      <c r="M64" s="38"/>
-      <c r="N64" s="38"/>
-      <c r="O64" s="39"/>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B64" s="43"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="45"/>
+      <c r="J64" s="43"/>
+      <c r="K64" s="44"/>
+      <c r="L64" s="44"/>
+      <c r="M64" s="44"/>
+      <c r="N64" s="44"/>
+      <c r="O64" s="45"/>
       <c r="W64" s="14"/>
       <c r="X64" s="14"/>
       <c r="Y64" s="14"/>
       <c r="Z64" s="14"/>
     </row>
     <row r="65" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B65" s="47"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="49"/>
-      <c r="J65" s="37"/>
-      <c r="K65" s="38"/>
-      <c r="L65" s="38"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="38"/>
-      <c r="O65" s="39"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="45"/>
+      <c r="J65" s="43"/>
+      <c r="K65" s="44"/>
+      <c r="L65" s="44"/>
+      <c r="M65" s="44"/>
+      <c r="N65" s="44"/>
+      <c r="O65" s="45"/>
       <c r="W65" s="14"/>
       <c r="X65" s="14"/>
       <c r="Y65" s="14"/>
       <c r="Z65" s="14"/>
     </row>
     <row r="66" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B66" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" s="43"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="43"/>
-      <c r="G66" s="44"/>
-      <c r="J66" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="K66" s="38"/>
-      <c r="L66" s="38"/>
-      <c r="M66" s="38"/>
-      <c r="N66" s="38"/>
-      <c r="O66" s="39"/>
+      <c r="B66" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" s="55"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="55"/>
+      <c r="G66" s="56"/>
+      <c r="J66" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="K66" s="44"/>
+      <c r="L66" s="44"/>
+      <c r="M66" s="44"/>
+      <c r="N66" s="44"/>
+      <c r="O66" s="45"/>
       <c r="W66" s="14"/>
       <c r="X66" s="14"/>
       <c r="Y66" s="14"/>
       <c r="Z66" s="14"/>
     </row>
     <row r="67" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B67" s="47"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="49"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="38"/>
-      <c r="L67" s="38"/>
-      <c r="M67" s="38"/>
-      <c r="N67" s="38"/>
-      <c r="O67" s="39"/>
+      <c r="B67" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="41"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="41"/>
+      <c r="G67" s="42"/>
+      <c r="J67" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="K67" s="44"/>
+      <c r="L67" s="44"/>
+      <c r="M67" s="44"/>
+      <c r="N67" s="44"/>
+      <c r="O67" s="45"/>
       <c r="W67" s="14"/>
       <c r="X67" s="14"/>
       <c r="Y67" s="14"/>
       <c r="Z67" s="14"/>
     </row>
     <row r="68" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B68" s="47"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="49"/>
-      <c r="J68" s="37"/>
-      <c r="K68" s="38"/>
-      <c r="L68" s="38"/>
-      <c r="M68" s="38"/>
-      <c r="N68" s="38"/>
-      <c r="O68" s="39"/>
+      <c r="B68" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C68" s="41"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="41"/>
+      <c r="G68" s="42"/>
+      <c r="J68" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="K68" s="44"/>
+      <c r="L68" s="44"/>
+      <c r="M68" s="44"/>
+      <c r="N68" s="44"/>
+      <c r="O68" s="45"/>
       <c r="W68" s="14"/>
       <c r="X68" s="14"/>
       <c r="Y68" s="14"/>
       <c r="Z68" s="14"/>
     </row>
     <row r="69" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B69" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="44"/>
-      <c r="J69" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="K69" s="38"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
-      <c r="O69" s="39"/>
-      <c r="W69" s="13"/>
-      <c r="X69" s="13"/>
-      <c r="Y69" s="13"/>
-      <c r="Z69" s="13"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="38"/>
+      <c r="E69" s="38"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="39"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="44"/>
+      <c r="L69" s="44"/>
+      <c r="M69" s="44"/>
+      <c r="N69" s="44"/>
+      <c r="O69" s="45"/>
+      <c r="W69" s="14"/>
+      <c r="X69" s="14"/>
+      <c r="Y69" s="14"/>
+      <c r="Z69" s="14"/>
     </row>
     <row r="70" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B70" s="37"/>
@@ -2201,30 +2213,34 @@
       <c r="E70" s="38"/>
       <c r="F70" s="38"/>
       <c r="G70" s="39"/>
-      <c r="J70" s="37"/>
-      <c r="K70" s="38"/>
-      <c r="L70" s="38"/>
-      <c r="M70" s="38"/>
-      <c r="N70" s="38"/>
-      <c r="O70" s="39"/>
+      <c r="J70" s="43"/>
+      <c r="K70" s="44"/>
+      <c r="L70" s="44"/>
+      <c r="M70" s="44"/>
+      <c r="N70" s="44"/>
+      <c r="O70" s="45"/>
       <c r="W70" s="14"/>
       <c r="X70" s="14"/>
       <c r="Y70" s="14"/>
       <c r="Z70" s="14"/>
     </row>
     <row r="71" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B71" s="37"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="38"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="39"/>
-      <c r="J71" s="37"/>
-      <c r="K71" s="38"/>
-      <c r="L71" s="38"/>
-      <c r="M71" s="38"/>
-      <c r="N71" s="38"/>
-      <c r="O71" s="39"/>
+      <c r="B71" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="57"/>
+      <c r="F71" s="57"/>
+      <c r="G71" s="58"/>
+      <c r="J71" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="K71" s="44"/>
+      <c r="L71" s="44"/>
+      <c r="M71" s="44"/>
+      <c r="N71" s="44"/>
+      <c r="O71" s="45"/>
       <c r="W71" s="14"/>
       <c r="X71" s="14"/>
       <c r="Y71" s="14"/>
@@ -2232,227 +2248,227 @@
     </row>
     <row r="72" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B72" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="43"/>
-      <c r="G72" s="44"/>
-      <c r="J72" s="37"/>
-      <c r="K72" s="38"/>
-      <c r="L72" s="38"/>
-      <c r="M72" s="38"/>
-      <c r="N72" s="38"/>
-      <c r="O72" s="39"/>
+        <v>54</v>
+      </c>
+      <c r="C72" s="41"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="42"/>
+      <c r="J72" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="44"/>
+      <c r="N72" s="44"/>
+      <c r="O72" s="45"/>
       <c r="W72" s="14"/>
       <c r="X72" s="14"/>
       <c r="Y72" s="14"/>
       <c r="Z72" s="14"/>
     </row>
     <row r="73" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B73" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="49"/>
-      <c r="J73" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="K73" s="38"/>
-      <c r="L73" s="38"/>
-      <c r="M73" s="38"/>
-      <c r="N73" s="38"/>
-      <c r="O73" s="39"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="39"/>
+      <c r="J73" s="43"/>
+      <c r="K73" s="44"/>
+      <c r="L73" s="44"/>
+      <c r="M73" s="44"/>
+      <c r="N73" s="44"/>
+      <c r="O73" s="45"/>
       <c r="W73" s="14"/>
       <c r="X73" s="14"/>
       <c r="Y73" s="14"/>
       <c r="Z73" s="14"/>
     </row>
     <row r="74" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B74" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74" s="58"/>
-      <c r="D74" s="58"/>
-      <c r="E74" s="58"/>
-      <c r="F74" s="58"/>
-      <c r="G74" s="59"/>
-      <c r="J74" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="K74" s="38"/>
-      <c r="L74" s="38"/>
-      <c r="M74" s="38"/>
-      <c r="N74" s="38"/>
-      <c r="O74" s="39"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="39"/>
+      <c r="J74" s="43"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="44"/>
+      <c r="M74" s="44"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="45"/>
       <c r="W74" s="14"/>
       <c r="X74" s="14"/>
       <c r="Y74" s="14"/>
       <c r="Z74" s="14"/>
     </row>
     <row r="75" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B75" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="59"/>
-      <c r="J75" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="K75" s="38"/>
-      <c r="L75" s="38"/>
-      <c r="M75" s="38"/>
-      <c r="N75" s="38"/>
-      <c r="O75" s="39"/>
-      <c r="W75" s="14"/>
-      <c r="X75" s="14"/>
-      <c r="Y75" s="14"/>
-      <c r="Z75" s="14"/>
+      <c r="B75" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="57"/>
+      <c r="F75" s="57"/>
+      <c r="G75" s="58"/>
+      <c r="J75" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K75" s="44"/>
+      <c r="L75" s="44"/>
+      <c r="M75" s="44"/>
+      <c r="N75" s="44"/>
+      <c r="O75" s="45"/>
+      <c r="W75" s="13"/>
+      <c r="X75" s="13"/>
+      <c r="Y75" s="13"/>
+      <c r="Z75" s="13"/>
     </row>
     <row r="76" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B76" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="58"/>
-      <c r="D76" s="58"/>
-      <c r="E76" s="58"/>
-      <c r="F76" s="58"/>
-      <c r="G76" s="59"/>
-      <c r="J76" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="K76" s="38"/>
-      <c r="L76" s="38"/>
-      <c r="M76" s="38"/>
-      <c r="N76" s="38"/>
-      <c r="O76" s="39"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="45"/>
+      <c r="J76" s="43"/>
+      <c r="K76" s="44"/>
+      <c r="L76" s="44"/>
+      <c r="M76" s="44"/>
+      <c r="N76" s="44"/>
+      <c r="O76" s="45"/>
       <c r="W76" s="14"/>
       <c r="X76" s="14"/>
       <c r="Y76" s="14"/>
       <c r="Z76" s="14"/>
     </row>
     <row r="77" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B77" s="47"/>
-      <c r="C77" s="48"/>
-      <c r="D77" s="48"/>
-      <c r="E77" s="48"/>
-      <c r="F77" s="48"/>
-      <c r="G77" s="49"/>
-      <c r="J77" s="37"/>
-      <c r="K77" s="38"/>
-      <c r="L77" s="38"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="38"/>
-      <c r="O77" s="39"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="45"/>
+      <c r="J77" s="43"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="44"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="44"/>
+      <c r="O77" s="45"/>
       <c r="W77" s="14"/>
       <c r="X77" s="14"/>
       <c r="Y77" s="14"/>
       <c r="Z77" s="14"/>
     </row>
     <row r="78" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B78" s="47"/>
-      <c r="C78" s="48"/>
-      <c r="D78" s="48"/>
-      <c r="E78" s="48"/>
-      <c r="F78" s="48"/>
-      <c r="G78" s="49"/>
-      <c r="J78" s="37"/>
-      <c r="K78" s="38"/>
-      <c r="L78" s="38"/>
-      <c r="M78" s="38"/>
-      <c r="N78" s="38"/>
-      <c r="O78" s="39"/>
+      <c r="B78" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="57"/>
+      <c r="D78" s="57"/>
+      <c r="E78" s="57"/>
+      <c r="F78" s="57"/>
+      <c r="G78" s="58"/>
+      <c r="J78" s="43"/>
+      <c r="K78" s="44"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="44"/>
+      <c r="N78" s="44"/>
+      <c r="O78" s="45"/>
       <c r="W78" s="14"/>
       <c r="X78" s="14"/>
       <c r="Y78" s="14"/>
       <c r="Z78" s="14"/>
     </row>
     <row r="79" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B79" s="47"/>
-      <c r="C79" s="48"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="49"/>
-      <c r="J79" s="37"/>
-      <c r="K79" s="38"/>
-      <c r="L79" s="38"/>
-      <c r="M79" s="38"/>
-      <c r="N79" s="38"/>
-      <c r="O79" s="39"/>
+      <c r="B79" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="38"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="39"/>
+      <c r="J79" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="K79" s="44"/>
+      <c r="L79" s="44"/>
+      <c r="M79" s="44"/>
+      <c r="N79" s="44"/>
+      <c r="O79" s="45"/>
       <c r="W79" s="14"/>
       <c r="X79" s="14"/>
       <c r="Y79" s="14"/>
       <c r="Z79" s="14"/>
     </row>
     <row r="80" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B80" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="38"/>
-      <c r="G80" s="39"/>
-      <c r="J80" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="K80" s="38"/>
-      <c r="L80" s="38"/>
-      <c r="M80" s="38"/>
-      <c r="N80" s="38"/>
-      <c r="O80" s="39"/>
-      <c r="W80" s="13"/>
-      <c r="X80" s="13"/>
-      <c r="Y80" s="13"/>
-      <c r="Z80" s="13"/>
+      <c r="B80" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" s="41"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
+      <c r="F80" s="41"/>
+      <c r="G80" s="42"/>
+      <c r="J80" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="K80" s="44"/>
+      <c r="L80" s="44"/>
+      <c r="M80" s="44"/>
+      <c r="N80" s="44"/>
+      <c r="O80" s="45"/>
+      <c r="W80" s="14"/>
+      <c r="X80" s="14"/>
+      <c r="Y80" s="14"/>
+      <c r="Z80" s="14"/>
     </row>
     <row r="81" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B81" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C81" s="38"/>
-      <c r="D81" s="38"/>
-      <c r="E81" s="38"/>
-      <c r="F81" s="38"/>
-      <c r="G81" s="39"/>
-      <c r="J81" s="37" t="s">
+      <c r="B81" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="41"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="42"/>
+      <c r="J81" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="K81" s="44"/>
+      <c r="L81" s="44"/>
+      <c r="M81" s="44"/>
+      <c r="N81" s="44"/>
+      <c r="O81" s="45"/>
+      <c r="W81" s="14"/>
+      <c r="X81" s="14"/>
+      <c r="Y81" s="14"/>
+      <c r="Z81" s="14"/>
+    </row>
+    <row r="82" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B82" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" s="41"/>
+      <c r="D82" s="41"/>
+      <c r="E82" s="41"/>
+      <c r="F82" s="41"/>
+      <c r="G82" s="42"/>
+      <c r="J82" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="K81" s="38"/>
-      <c r="L81" s="38"/>
-      <c r="M81" s="38"/>
-      <c r="N81" s="38"/>
-      <c r="O81" s="39"/>
-      <c r="W81" s="13"/>
-      <c r="X81" s="13"/>
-      <c r="Y81" s="13"/>
-      <c r="Z81" s="13"/>
-    </row>
-    <row r="82" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B82" s="37"/>
-      <c r="C82" s="38"/>
-      <c r="D82" s="38"/>
-      <c r="E82" s="38"/>
-      <c r="F82" s="38"/>
-      <c r="G82" s="39"/>
-      <c r="J82" s="37"/>
-      <c r="K82" s="38"/>
-      <c r="L82" s="38"/>
-      <c r="M82" s="38"/>
-      <c r="N82" s="38"/>
-      <c r="O82" s="39"/>
-      <c r="W82" s="13"/>
-      <c r="X82" s="13"/>
-      <c r="Y82" s="13"/>
-      <c r="Z82" s="13"/>
+      <c r="K82" s="44"/>
+      <c r="L82" s="44"/>
+      <c r="M82" s="44"/>
+      <c r="N82" s="44"/>
+      <c r="O82" s="45"/>
+      <c r="W82" s="14"/>
+      <c r="X82" s="14"/>
+      <c r="Y82" s="14"/>
+      <c r="Z82" s="14"/>
     </row>
     <row r="83" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B83" s="37"/>
@@ -2461,207 +2477,295 @@
       <c r="E83" s="38"/>
       <c r="F83" s="38"/>
       <c r="G83" s="39"/>
-      <c r="J83" s="37"/>
-      <c r="K83" s="38"/>
-      <c r="L83" s="38"/>
-      <c r="M83" s="38"/>
-      <c r="N83" s="38"/>
-      <c r="O83" s="39"/>
-      <c r="W83" s="13"/>
-      <c r="X83" s="13"/>
-      <c r="Y83" s="13"/>
-      <c r="Z83" s="13"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="44"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="44"/>
+      <c r="O83" s="45"/>
+      <c r="W83" s="14"/>
+      <c r="X83" s="14"/>
+      <c r="Y83" s="14"/>
+      <c r="Z83" s="14"/>
     </row>
     <row r="84" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B84" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C84" s="43"/>
-      <c r="D84" s="43"/>
-      <c r="E84" s="43"/>
-      <c r="F84" s="43"/>
-      <c r="G84" s="44"/>
-      <c r="J84" s="37"/>
-      <c r="K84" s="38"/>
-      <c r="L84" s="38"/>
-      <c r="M84" s="38"/>
-      <c r="N84" s="38"/>
-      <c r="O84" s="39"/>
-      <c r="W84" s="13"/>
-      <c r="X84" s="13"/>
-      <c r="Y84" s="13"/>
-      <c r="Z84" s="13"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="39"/>
+      <c r="J84" s="43"/>
+      <c r="K84" s="44"/>
+      <c r="L84" s="44"/>
+      <c r="M84" s="44"/>
+      <c r="N84" s="44"/>
+      <c r="O84" s="45"/>
+      <c r="W84" s="14"/>
+      <c r="X84" s="14"/>
+      <c r="Y84" s="14"/>
+      <c r="Z84" s="14"/>
     </row>
     <row r="85" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B85" s="37" t="s">
-        <v>24</v>
-      </c>
+      <c r="B85" s="37"/>
       <c r="C85" s="38"/>
       <c r="D85" s="38"/>
       <c r="E85" s="38"/>
       <c r="F85" s="38"/>
       <c r="G85" s="39"/>
-      <c r="J85" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K85" s="38"/>
-      <c r="L85" s="38"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
-      <c r="O85" s="39"/>
-      <c r="W85" s="13"/>
-      <c r="X85" s="13"/>
-      <c r="Y85" s="13"/>
-      <c r="Z85" s="13"/>
+      <c r="J85" s="43"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="44"/>
+      <c r="M85" s="44"/>
+      <c r="N85" s="44"/>
+      <c r="O85" s="45"/>
+      <c r="W85" s="14"/>
+      <c r="X85" s="14"/>
+      <c r="Y85" s="14"/>
+      <c r="Z85" s="14"/>
     </row>
     <row r="86" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B86" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="39"/>
-      <c r="J86" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="K86" s="38"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="38"/>
-      <c r="O86" s="39"/>
+      <c r="B86" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="45"/>
+      <c r="J86" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="K86" s="44"/>
+      <c r="L86" s="44"/>
+      <c r="M86" s="44"/>
+      <c r="N86" s="44"/>
+      <c r="O86" s="45"/>
       <c r="W86" s="13"/>
       <c r="X86" s="13"/>
       <c r="Y86" s="13"/>
       <c r="Z86" s="13"/>
     </row>
     <row r="87" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B87" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="39"/>
-      <c r="J87" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="K87" s="38"/>
-      <c r="L87" s="38"/>
-      <c r="M87" s="38"/>
-      <c r="N87" s="38"/>
-      <c r="O87" s="39"/>
+      <c r="B87" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="45"/>
+      <c r="J87" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K87" s="44"/>
+      <c r="L87" s="44"/>
+      <c r="M87" s="44"/>
+      <c r="N87" s="44"/>
+      <c r="O87" s="45"/>
       <c r="W87" s="13"/>
       <c r="X87" s="13"/>
       <c r="Y87" s="13"/>
       <c r="Z87" s="13"/>
     </row>
     <row r="88" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B88" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="C88" s="38"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="39"/>
-      <c r="J88" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="K88" s="38"/>
-      <c r="L88" s="38"/>
-      <c r="M88" s="38"/>
-      <c r="N88" s="38"/>
-      <c r="O88" s="39"/>
-      <c r="W88" s="15"/>
+      <c r="B88" s="43"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="45"/>
+      <c r="J88" s="43"/>
+      <c r="K88" s="44"/>
+      <c r="L88" s="44"/>
+      <c r="M88" s="44"/>
+      <c r="N88" s="44"/>
+      <c r="O88" s="45"/>
+      <c r="W88" s="13"/>
       <c r="X88" s="13"/>
       <c r="Y88" s="13"/>
       <c r="Z88" s="13"/>
     </row>
     <row r="89" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="W89" s="14"/>
-      <c r="X89" s="14"/>
-      <c r="Y89" s="14"/>
-      <c r="Z89" s="14"/>
+      <c r="B89" s="43"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="45"/>
+      <c r="J89" s="43"/>
+      <c r="K89" s="44"/>
+      <c r="L89" s="44"/>
+      <c r="M89" s="44"/>
+      <c r="N89" s="44"/>
+      <c r="O89" s="45"/>
+      <c r="W89" s="13"/>
+      <c r="X89" s="13"/>
+      <c r="Y89" s="13"/>
+      <c r="Z89" s="13"/>
     </row>
     <row r="90" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="W90" s="14"/>
-      <c r="X90" s="14"/>
-      <c r="Y90" s="14"/>
-      <c r="Z90" s="14"/>
+      <c r="B90" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="57"/>
+      <c r="F90" s="57"/>
+      <c r="G90" s="58"/>
+      <c r="J90" s="43"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="44"/>
+      <c r="M90" s="44"/>
+      <c r="N90" s="44"/>
+      <c r="O90" s="45"/>
+      <c r="W90" s="13"/>
+      <c r="X90" s="13"/>
+      <c r="Y90" s="13"/>
+      <c r="Z90" s="13"/>
+    </row>
+    <row r="91" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B91" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="45"/>
+      <c r="J91" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="K91" s="44"/>
+      <c r="L91" s="44"/>
+      <c r="M91" s="44"/>
+      <c r="N91" s="44"/>
+      <c r="O91" s="45"/>
+      <c r="W91" s="13"/>
+      <c r="X91" s="13"/>
+      <c r="Y91" s="13"/>
+      <c r="Z91" s="13"/>
+    </row>
+    <row r="92" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B92" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="45"/>
+      <c r="J92" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="K92" s="44"/>
+      <c r="L92" s="44"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="44"/>
+      <c r="O92" s="45"/>
+      <c r="W92" s="13"/>
+      <c r="X92" s="13"/>
+      <c r="Y92" s="13"/>
+      <c r="Z92" s="13"/>
+    </row>
+    <row r="93" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B93" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="45"/>
+      <c r="J93" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="K93" s="44"/>
+      <c r="L93" s="44"/>
+      <c r="M93" s="44"/>
+      <c r="N93" s="44"/>
+      <c r="O93" s="45"/>
+      <c r="W93" s="13"/>
+      <c r="X93" s="13"/>
+      <c r="Y93" s="13"/>
+      <c r="Z93" s="13"/>
+    </row>
+    <row r="94" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B94" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="45"/>
+      <c r="J94" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="K94" s="44"/>
+      <c r="L94" s="44"/>
+      <c r="M94" s="44"/>
+      <c r="N94" s="44"/>
+      <c r="O94" s="45"/>
+      <c r="W94" s="15"/>
+      <c r="X94" s="13"/>
+      <c r="Y94" s="13"/>
+      <c r="Z94" s="13"/>
+    </row>
+    <row r="95" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="W95" s="14"/>
+      <c r="X95" s="14"/>
+      <c r="Y95" s="14"/>
+      <c r="Z95" s="14"/>
+    </row>
+    <row r="96" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="W96" s="14"/>
+      <c r="X96" s="14"/>
+      <c r="Y96" s="14"/>
+      <c r="Z96" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="123">
-    <mergeCell ref="B79:G79"/>
+  <mergeCells count="132">
+    <mergeCell ref="J92:O92"/>
+    <mergeCell ref="B86:G86"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:G88"/>
+    <mergeCell ref="B91:G91"/>
     <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B74:G74"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="J79:O79"/>
-    <mergeCell ref="J78:O78"/>
-    <mergeCell ref="J77:O77"/>
-    <mergeCell ref="J76:O76"/>
-    <mergeCell ref="J75:O75"/>
-    <mergeCell ref="J74:O74"/>
-    <mergeCell ref="J73:O73"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="J58:O58"/>
-    <mergeCell ref="J59:O59"/>
-    <mergeCell ref="J60:O60"/>
-    <mergeCell ref="J61:O61"/>
-    <mergeCell ref="J62:O62"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B61:G61"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="B71:G71"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="J67:O67"/>
-    <mergeCell ref="J65:O65"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="B67:G67"/>
     <mergeCell ref="B68:G68"/>
-    <mergeCell ref="J64:O64"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B53:G53"/>
-    <mergeCell ref="J56:O56"/>
-    <mergeCell ref="J53:O53"/>
-    <mergeCell ref="J55:O55"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="J67:O67"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="J94:O94"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="J66:O66"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="J75:O75"/>
+    <mergeCell ref="J76:O76"/>
+    <mergeCell ref="J77:O77"/>
+    <mergeCell ref="J86:O86"/>
+    <mergeCell ref="J87:O87"/>
+    <mergeCell ref="J88:O88"/>
+    <mergeCell ref="J93:O93"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B71:G71"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="J91:O91"/>
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F4:G4"/>
@@ -2669,56 +2773,93 @@
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:D6"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="J90:O90"/>
+    <mergeCell ref="J89:O89"/>
+    <mergeCell ref="J60:O60"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="J52:O52"/>
+    <mergeCell ref="J53:O53"/>
+    <mergeCell ref="J54:O54"/>
+    <mergeCell ref="J55:O55"/>
+    <mergeCell ref="J57:O57"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="L6:M40"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="J56:O56"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="J78:O78"/>
+    <mergeCell ref="J61:O61"/>
+    <mergeCell ref="J62:O62"/>
+    <mergeCell ref="J63:O63"/>
+    <mergeCell ref="J64:O64"/>
+    <mergeCell ref="J65:O65"/>
+    <mergeCell ref="B61:G61"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="J74:O74"/>
+    <mergeCell ref="J73:O73"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B70:G70"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="B84:G84"/>
     <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="J85:O85"/>
     <mergeCell ref="J84:O84"/>
     <mergeCell ref="J83:O83"/>
-    <mergeCell ref="J57:O57"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="J50:O50"/>
-    <mergeCell ref="J51:O51"/>
-    <mergeCell ref="J52:O52"/>
-    <mergeCell ref="J54:O54"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="L6:M37"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="J88:O88"/>
-    <mergeCell ref="B86:G86"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:G88"/>
-    <mergeCell ref="J63:O63"/>
-    <mergeCell ref="J66:O66"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="J82:O82"/>
+    <mergeCell ref="J81:O81"/>
     <mergeCell ref="J80:O80"/>
-    <mergeCell ref="J81:O81"/>
-    <mergeCell ref="J82:O82"/>
-    <mergeCell ref="J87:O87"/>
-    <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="J85:O85"/>
-    <mergeCell ref="J86:O86"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B82:G82"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="J79:O79"/>
   </mergeCells>
-  <conditionalFormatting sqref="I21:J21">
+  <conditionalFormatting sqref="I23:J23">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -2730,7 +2871,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
+  <conditionalFormatting sqref="H24">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -2742,7 +2883,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
+  <conditionalFormatting sqref="H25:H26">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -2754,7 +2895,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
+  <conditionalFormatting sqref="H27">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -2766,7 +2907,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
+  <conditionalFormatting sqref="K23">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -2790,7 +2931,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:G20">
+  <conditionalFormatting sqref="F20:G22">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3018,7 +3159,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I19 I17">
+  <conditionalFormatting sqref="I17 I19">
     <cfRule type="colorScale" priority="208">
       <colorScale>
         <cfvo type="min"/>
@@ -3042,7 +3183,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K24 A22:D22 E25:K25 A27:J27 E26:J26 E21:H24 A23 A25 J22:J24 A5:E5 E6:L6 A19:E20 H7:K7 E7:F9 I8:K8 H9 J9:K9 J13 K11 N6:N9 J15:J17 J19 H15:H17 H19 E15:F18 N13 H13 E13:F13 N11 H11 E11:F11 A29:A30 N15:N19 E29:K30 A31:K31 A37:K37 E32:K36 A36 A28:K28">
+  <conditionalFormatting sqref="K23:K27 A24:D24 E28:K28 A30:J30 E29:J29 E23:H27 A25:A26 A28 J24:J27 A5:E5 E6:L6 A19:E20 H7:K7 E7:F9 I8:K8 H9 J9:K9 J13 K11 N6:N9 J15:J17 J19 H15:H17 H19 E15:F18 N13 H13 E13:F13 N11 H11 E11:F11 A32:A33 N15:N19 E32:K33 A34:K34 A40:K40 E35:K39 A39 A31:K31 A21:A22 E21:E22">
     <cfRule type="colorScale" priority="229">
       <colorScale>
         <cfvo type="min"/>
@@ -3102,43 +3243,43 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A38">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A34">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3162,7 +3303,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28">
+  <conditionalFormatting sqref="N31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Documentatie: Planning + Taakverdeling + Rolverdeling.xlsx aangepast.
</commit_message>
<xml_diff>
--- a/Documentatie/Planning + Taakverdeling + Rolverdeling/Planning + Taakverdeling + Rolverdeling.xlsx
+++ b/Documentatie/Planning + Taakverdeling + Rolverdeling/Planning + Taakverdeling + Rolverdeling.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="82">
   <si>
     <t>Onderdeel:</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>Jeffrey</t>
+  </si>
+  <si>
+    <t>Melinda en Arjen (Joshua, Remco, Jeffrey en Yme)</t>
   </si>
 </sst>
 </file>
@@ -756,6 +759,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,44 +789,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1135,13 +1138,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
       <c r="G2" s="55" t="s">
         <v>6</v>
       </c>
@@ -1164,32 +1167,32 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="46" t="s">
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="16">
         <v>46</v>
       </c>
@@ -1222,910 +1225,910 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
       <c r="G7" s="35"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="56" t="s">
+      <c r="M7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="56"/>
+      <c r="N7" s="51"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
       <c r="G8" s="26"/>
       <c r="H8" s="35"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="26"/>
       <c r="H9" s="2"/>
       <c r="I9" s="35"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="56"/>
-      <c r="N9" s="56"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="26"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="35"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
       <c r="G11" s="26"/>
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
       <c r="J11" s="35"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="26"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="35"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="26"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="35"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
       <c r="G14" s="26"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="35"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
       <c r="G15" s="26"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="3"/>
       <c r="L15" s="35"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
       <c r="O16" s="9"/>
       <c r="P16" s="35"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
       <c r="G17" s="26"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
       <c r="O17" s="3"/>
       <c r="P17" s="35"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
       <c r="G18" s="26"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
       <c r="G19" s="26"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="9"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="35"/>
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="26"/>
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="9"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="35"/>
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
       <c r="G21" s="26"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
       <c r="G22" s="26"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
       <c r="G23" s="2"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
       <c r="O23" s="9"/>
       <c r="P23" s="35"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
       <c r="G24" s="2"/>
       <c r="H24" s="3"/>
       <c r="I24" s="4"/>
       <c r="J24" s="12"/>
       <c r="K24" s="32"/>
       <c r="L24" s="32"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
+      <c r="M24" s="51"/>
+      <c r="N24" s="51"/>
       <c r="O24" s="32"/>
       <c r="P24" s="32"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
       <c r="G25" s="2"/>
       <c r="H25" s="3"/>
       <c r="I25" s="4"/>
       <c r="J25" s="12"/>
       <c r="K25" s="32"/>
       <c r="L25" s="32"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
       <c r="O25" s="32"/>
       <c r="P25" s="32"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
       <c r="G26" s="2"/>
       <c r="H26" s="3"/>
       <c r="I26" s="4"/>
       <c r="J26" s="9"/>
       <c r="K26" s="32"/>
       <c r="L26" s="32"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="56"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
       <c r="O26" s="32"/>
       <c r="P26" s="32"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
       <c r="J27" s="4"/>
       <c r="K27" s="12"/>
       <c r="L27" s="32"/>
-      <c r="M27" s="56"/>
-      <c r="N27" s="56"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
       <c r="O27" s="32"/>
       <c r="P27" s="32"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="32"/>
       <c r="L28" s="32"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="10"/>
       <c r="L29" s="11"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
       <c r="O29" s="12"/>
       <c r="P29" s="32"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="26"/>
       <c r="J30" s="32"/>
       <c r="K30" s="32"/>
       <c r="L30" s="32"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
       <c r="O30" s="32"/>
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="26"/>
       <c r="J31" s="32"/>
       <c r="K31" s="32"/>
       <c r="L31" s="32"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
       <c r="O31" s="32"/>
       <c r="P31" s="32"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="2"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
       <c r="L32" s="11"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="56"/>
+      <c r="M32" s="51"/>
+      <c r="N32" s="51"/>
       <c r="O32" s="12"/>
       <c r="P32" s="36"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
       <c r="G33" s="2"/>
       <c r="H33" s="3"/>
       <c r="I33" s="4"/>
       <c r="J33" s="12"/>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
-      <c r="M33" s="56"/>
-      <c r="N33" s="56"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
       <c r="G34" s="2"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="11"/>
       <c r="K34" s="12"/>
       <c r="L34" s="32"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="56"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="51"/>
       <c r="O34" s="32"/>
       <c r="P34" s="32"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="26"/>
       <c r="J35" s="32"/>
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
-      <c r="M35" s="56"/>
-      <c r="N35" s="56"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
       <c r="O35" s="32"/>
       <c r="P35" s="32"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="29"/>
       <c r="J36" s="30"/>
       <c r="K36" s="31"/>
       <c r="L36" s="33"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="44" t="s">
+      <c r="B37" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
       <c r="G37" s="2"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="10"/>
       <c r="L37" s="11"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
       <c r="O37" s="12"/>
       <c r="P37" s="36"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
       <c r="G38" s="2"/>
       <c r="H38" s="3"/>
       <c r="I38" s="4"/>
       <c r="J38" s="9"/>
       <c r="K38" s="32"/>
       <c r="L38" s="32"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
       <c r="O38" s="33"/>
       <c r="P38" s="33"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
       <c r="G39" s="2"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="11"/>
       <c r="L39" s="12"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
       <c r="O39" s="33"/>
       <c r="P39" s="33"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" s="43" t="s">
+      <c r="B40" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
       <c r="G40" s="2"/>
       <c r="H40" s="3"/>
       <c r="I40" s="4"/>
       <c r="J40" s="9"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="56"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
       <c r="O40" s="33"/>
       <c r="P40" s="33"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="56"/>
-      <c r="N41" s="56"/>
+      <c r="M41" s="51"/>
+      <c r="N41" s="51"/>
       <c r="O41" s="12"/>
       <c r="P41" s="33"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B42" s="43" t="s">
+      <c r="B42" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
       <c r="G42" s="2"/>
       <c r="H42" s="3"/>
       <c r="I42" s="4"/>
       <c r="J42" s="9"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
-      <c r="M42" s="56"/>
-      <c r="N42" s="56"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
       <c r="O42" s="33"/>
       <c r="P42" s="33"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" s="43" t="s">
+      <c r="B43" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
       <c r="G43" s="2"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
-      <c r="M43" s="56"/>
-      <c r="N43" s="56"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="51"/>
       <c r="O43" s="11"/>
       <c r="P43" s="12"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="26"/>
       <c r="J44" s="26"/>
       <c r="K44" s="32"/>
       <c r="L44" s="32"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
       <c r="O44" s="33"/>
       <c r="P44" s="33"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="26"/>
       <c r="J45" s="26"/>
       <c r="K45" s="26"/>
       <c r="L45" s="26"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="51"/>
       <c r="O45" s="27"/>
       <c r="P45" s="28"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
       <c r="G46" s="2"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="10"/>
       <c r="L46" s="11"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="51"/>
       <c r="O46" s="12"/>
       <c r="P46" s="36"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="3"/>
       <c r="J47" s="4"/>
       <c r="K47" s="9"/>
       <c r="L47" s="26"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
       <c r="O47" s="33"/>
       <c r="P47" s="33"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="3"/>
       <c r="J48" s="4"/>
       <c r="K48" s="9"/>
       <c r="L48" s="26"/>
-      <c r="M48" s="56"/>
-      <c r="N48" s="56"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="51"/>
       <c r="O48" s="33"/>
       <c r="P48" s="33"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="3"/>
       <c r="J49" s="4"/>
       <c r="K49" s="9"/>
       <c r="L49" s="26"/>
-      <c r="M49" s="56"/>
-      <c r="N49" s="56"/>
+      <c r="M49" s="51"/>
+      <c r="N49" s="51"/>
       <c r="O49" s="33"/>
       <c r="P49" s="33"/>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="26"/>
       <c r="J50" s="26"/>
       <c r="K50" s="26"/>
       <c r="L50" s="26"/>
-      <c r="M50" s="56"/>
-      <c r="N50" s="56"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="51"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="26"/>
       <c r="J51" s="26"/>
       <c r="K51" s="29"/>
       <c r="L51" s="29"/>
-      <c r="M51" s="56"/>
-      <c r="N51" s="56"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="51"/>
       <c r="O51" s="31"/>
       <c r="P51" s="28"/>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
+      <c r="C52" s="52"/>
+      <c r="D52" s="52"/>
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="51"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B53" s="45" t="s">
+      <c r="B53" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
       <c r="G53" s="3"/>
       <c r="H53" s="35"/>
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
       <c r="K53" s="26"/>
       <c r="L53" s="26"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="56"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="51"/>
       <c r="O53" s="31"/>
       <c r="P53" s="28"/>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B54" s="45" t="s">
+      <c r="B54" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="45"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
       <c r="G54" s="3"/>
       <c r="H54" s="35"/>
       <c r="I54" s="26"/>
       <c r="J54" s="26"/>
       <c r="K54" s="26"/>
       <c r="L54" s="26"/>
-      <c r="M54" s="56"/>
-      <c r="N54" s="56"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="51"/>
       <c r="O54" s="31"/>
       <c r="P54" s="28"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B55" s="45" t="s">
+      <c r="B55" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
       <c r="G55" s="3"/>
       <c r="H55" s="35"/>
       <c r="I55" s="26"/>
       <c r="J55" s="26"/>
       <c r="K55" s="26"/>
       <c r="L55" s="26"/>
-      <c r="M55" s="56"/>
-      <c r="N55" s="56"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="51"/>
       <c r="O55" s="27"/>
       <c r="P55" s="28"/>
       <c r="R55" t="s">
@@ -2133,186 +2136,186 @@
       </c>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B56" s="45" t="s">
+      <c r="B56" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
       <c r="G56" s="26"/>
       <c r="H56" s="3"/>
       <c r="I56" s="35"/>
       <c r="J56" s="26"/>
       <c r="K56" s="26"/>
       <c r="L56" s="26"/>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="51"/>
       <c r="O56" s="27"/>
       <c r="P56" s="28"/>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B57" s="45" t="s">
+      <c r="B57" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
       <c r="G57" s="26"/>
       <c r="H57" s="26"/>
       <c r="I57" s="3"/>
       <c r="J57" s="35"/>
       <c r="K57" s="26"/>
       <c r="L57" s="26"/>
-      <c r="M57" s="56"/>
-      <c r="N57" s="56"/>
+      <c r="M57" s="51"/>
+      <c r="N57" s="51"/>
       <c r="O57" s="27"/>
       <c r="P57" s="28"/>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B58" s="45" t="s">
+      <c r="B58" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
       <c r="G58" s="26"/>
       <c r="H58" s="26"/>
       <c r="I58" s="3"/>
       <c r="J58" s="35"/>
       <c r="K58" s="26"/>
       <c r="L58" s="26"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="51"/>
       <c r="O58" s="27"/>
       <c r="P58" s="28"/>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B59" s="45" t="s">
+      <c r="B59" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
       <c r="G59" s="26"/>
       <c r="H59" s="26"/>
       <c r="I59" s="26"/>
       <c r="J59" s="3"/>
       <c r="K59" s="35"/>
       <c r="L59" s="26"/>
-      <c r="M59" s="56"/>
-      <c r="N59" s="56"/>
+      <c r="M59" s="51"/>
+      <c r="N59" s="51"/>
       <c r="O59" s="27"/>
       <c r="P59" s="28"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B60" s="45" t="s">
+      <c r="B60" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45"/>
-      <c r="E60" s="45"/>
-      <c r="F60" s="45"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
       <c r="G60" s="26"/>
       <c r="H60" s="26"/>
       <c r="I60" s="26"/>
       <c r="J60" s="26"/>
       <c r="K60" s="3"/>
       <c r="L60" s="35"/>
-      <c r="M60" s="56"/>
-      <c r="N60" s="56"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="51"/>
       <c r="O60" s="27"/>
       <c r="P60" s="28"/>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B61" s="45" t="s">
+      <c r="B61" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="45"/>
-      <c r="F61" s="45"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
       <c r="G61" s="26"/>
       <c r="H61" s="26"/>
       <c r="I61" s="26"/>
       <c r="J61" s="26"/>
       <c r="K61" s="3"/>
       <c r="L61" s="35"/>
-      <c r="M61" s="56"/>
-      <c r="N61" s="56"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="51"/>
       <c r="O61" s="27"/>
       <c r="P61" s="28"/>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B62" s="45"/>
-      <c r="C62" s="45"/>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45"/>
-      <c r="F62" s="45"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
       <c r="G62" s="26"/>
       <c r="H62" s="26"/>
       <c r="I62" s="26"/>
       <c r="J62" s="26"/>
       <c r="K62" s="26"/>
       <c r="L62" s="26"/>
-      <c r="M62" s="56"/>
-      <c r="N62" s="56"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="51"/>
       <c r="O62" s="27"/>
       <c r="P62" s="28"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B63" s="45"/>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
       <c r="G63" s="26"/>
       <c r="H63" s="26"/>
       <c r="I63" s="26"/>
       <c r="J63" s="26"/>
       <c r="K63" s="26"/>
       <c r="L63" s="26"/>
-      <c r="M63" s="56"/>
-      <c r="N63" s="56"/>
+      <c r="M63" s="51"/>
+      <c r="N63" s="51"/>
       <c r="O63" s="27"/>
       <c r="P63" s="28"/>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B64" s="45"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
-      <c r="F64" s="45"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
       <c r="G64" s="26"/>
       <c r="H64" s="26"/>
       <c r="I64" s="26"/>
       <c r="J64" s="26"/>
       <c r="K64" s="26"/>
       <c r="L64" s="26"/>
-      <c r="M64" s="56"/>
-      <c r="N64" s="56"/>
+      <c r="M64" s="51"/>
+      <c r="N64" s="51"/>
       <c r="O64" s="27"/>
       <c r="P64" s="28"/>
     </row>
     <row r="65" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B65" s="45" t="s">
+      <c r="B65" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="45"/>
-      <c r="D65" s="45"/>
-      <c r="E65" s="45"/>
-      <c r="F65" s="45"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="50"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
-      <c r="M65" s="56"/>
-      <c r="N65" s="56"/>
+      <c r="M65" s="51"/>
+      <c r="N65" s="51"/>
       <c r="O65" s="35"/>
       <c r="P65" s="28"/>
       <c r="R65" t="s">
@@ -2320,21 +2323,21 @@
       </c>
     </row>
     <row r="66" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-      <c r="F66" s="45"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="4"/>
       <c r="L66" s="9"/>
-      <c r="M66" s="56"/>
-      <c r="N66" s="56"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="51"/>
       <c r="O66" s="36"/>
       <c r="P66" s="28"/>
       <c r="R66" t="s">
@@ -2371,14 +2374,14 @@
       <c r="O69" s="55"/>
     </row>
     <row r="75" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B75" s="47" t="s">
+      <c r="B75" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="54"/>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
@@ -2388,376 +2391,376 @@
       <c r="F76" s="8"/>
     </row>
     <row r="78" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B78" s="46" t="s">
+      <c r="B78" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C78" s="46"/>
-      <c r="D78" s="46"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="46"/>
-      <c r="G78" s="46"/>
-      <c r="K78" s="46" t="s">
+      <c r="C78" s="56"/>
+      <c r="D78" s="56"/>
+      <c r="E78" s="56"/>
+      <c r="F78" s="56"/>
+      <c r="G78" s="56"/>
+      <c r="K78" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="L78" s="46"/>
-      <c r="M78" s="46"/>
-      <c r="N78" s="46"/>
-      <c r="O78" s="46"/>
-      <c r="P78" s="46"/>
+      <c r="L78" s="56"/>
+      <c r="M78" s="56"/>
+      <c r="N78" s="56"/>
+      <c r="O78" s="56"/>
+      <c r="P78" s="56"/>
     </row>
     <row r="79" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B79" s="40" t="s">
+      <c r="B79" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C79" s="41"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
-      <c r="F79" s="41"/>
-      <c r="G79" s="42"/>
-      <c r="K79" s="40" t="s">
+      <c r="C79" s="47"/>
+      <c r="D79" s="47"/>
+      <c r="E79" s="47"/>
+      <c r="F79" s="47"/>
+      <c r="G79" s="48"/>
+      <c r="K79" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L79" s="41"/>
-      <c r="M79" s="41"/>
-      <c r="N79" s="41"/>
-      <c r="O79" s="41"/>
-      <c r="P79" s="42"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="47"/>
+      <c r="O79" s="47"/>
+      <c r="P79" s="48"/>
     </row>
     <row r="80" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B80" s="40" t="s">
+      <c r="B80" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C80" s="41"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="41"/>
-      <c r="F80" s="41"/>
-      <c r="G80" s="42"/>
-      <c r="K80" s="40" t="s">
+      <c r="C80" s="47"/>
+      <c r="D80" s="47"/>
+      <c r="E80" s="47"/>
+      <c r="F80" s="47"/>
+      <c r="G80" s="48"/>
+      <c r="K80" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L80" s="41"/>
-      <c r="M80" s="41"/>
-      <c r="N80" s="41"/>
-      <c r="O80" s="41"/>
-      <c r="P80" s="42"/>
+      <c r="L80" s="47"/>
+      <c r="M80" s="47"/>
+      <c r="N80" s="47"/>
+      <c r="O80" s="47"/>
+      <c r="P80" s="48"/>
       <c r="X80" s="13"/>
       <c r="Y80" s="13"/>
       <c r="Z80" s="13"/>
       <c r="AA80" s="13"/>
     </row>
     <row r="81" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B81" s="40" t="s">
+      <c r="B81" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C81" s="41"/>
-      <c r="D81" s="41"/>
-      <c r="E81" s="41"/>
-      <c r="F81" s="41"/>
-      <c r="G81" s="42"/>
-      <c r="K81" s="40" t="s">
+      <c r="C81" s="47"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="48"/>
+      <c r="K81" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L81" s="41"/>
-      <c r="M81" s="41"/>
-      <c r="N81" s="41"/>
-      <c r="O81" s="41"/>
-      <c r="P81" s="42"/>
+      <c r="L81" s="47"/>
+      <c r="M81" s="47"/>
+      <c r="N81" s="47"/>
+      <c r="O81" s="47"/>
+      <c r="P81" s="48"/>
       <c r="X81" s="14"/>
       <c r="Y81" s="14"/>
       <c r="Z81" s="14"/>
       <c r="AA81" s="14"/>
     </row>
     <row r="82" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B82" s="40" t="s">
+      <c r="B82" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="41"/>
-      <c r="D82" s="41"/>
-      <c r="E82" s="41"/>
-      <c r="F82" s="41"/>
-      <c r="G82" s="42"/>
-      <c r="K82" s="40" t="s">
+      <c r="C82" s="47"/>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="48"/>
+      <c r="K82" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L82" s="41"/>
-      <c r="M82" s="41"/>
-      <c r="N82" s="41"/>
-      <c r="O82" s="41"/>
-      <c r="P82" s="42"/>
+      <c r="L82" s="47"/>
+      <c r="M82" s="47"/>
+      <c r="N82" s="47"/>
+      <c r="O82" s="47"/>
+      <c r="P82" s="48"/>
       <c r="X82" s="14"/>
       <c r="Y82" s="14"/>
       <c r="Z82" s="14"/>
       <c r="AA82" s="14"/>
     </row>
     <row r="83" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B83" s="40" t="s">
+      <c r="B83" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C83" s="41"/>
-      <c r="D83" s="41"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="41"/>
-      <c r="G83" s="42"/>
-      <c r="K83" s="40" t="s">
+      <c r="C83" s="47"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="48"/>
+      <c r="K83" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L83" s="41"/>
-      <c r="M83" s="41"/>
-      <c r="N83" s="41"/>
-      <c r="O83" s="41"/>
-      <c r="P83" s="42"/>
+      <c r="L83" s="47"/>
+      <c r="M83" s="47"/>
+      <c r="N83" s="47"/>
+      <c r="O83" s="47"/>
+      <c r="P83" s="48"/>
       <c r="X83" s="14"/>
       <c r="Y83" s="14"/>
       <c r="Z83" s="14"/>
       <c r="AA83" s="14"/>
     </row>
     <row r="84" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="41"/>
-      <c r="D84" s="41"/>
-      <c r="E84" s="41"/>
-      <c r="F84" s="41"/>
-      <c r="G84" s="42"/>
-      <c r="K84" s="40" t="s">
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="48"/>
+      <c r="K84" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L84" s="41"/>
-      <c r="M84" s="41"/>
-      <c r="N84" s="41"/>
-      <c r="O84" s="41"/>
-      <c r="P84" s="42"/>
+      <c r="L84" s="47"/>
+      <c r="M84" s="47"/>
+      <c r="N84" s="47"/>
+      <c r="O84" s="47"/>
+      <c r="P84" s="48"/>
       <c r="X84" s="14"/>
       <c r="Y84" s="14"/>
       <c r="Z84" s="14"/>
       <c r="AA84" s="14"/>
     </row>
     <row r="85" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B85" s="40" t="s">
+      <c r="B85" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C85" s="41"/>
-      <c r="D85" s="41"/>
-      <c r="E85" s="41"/>
-      <c r="F85" s="41"/>
-      <c r="G85" s="42"/>
-      <c r="K85" s="40" t="s">
+      <c r="C85" s="47"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="47"/>
+      <c r="G85" s="48"/>
+      <c r="K85" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L85" s="41"/>
-      <c r="M85" s="41"/>
-      <c r="N85" s="41"/>
-      <c r="O85" s="41"/>
-      <c r="P85" s="42"/>
+      <c r="L85" s="47"/>
+      <c r="M85" s="47"/>
+      <c r="N85" s="47"/>
+      <c r="O85" s="47"/>
+      <c r="P85" s="48"/>
       <c r="X85" s="14"/>
       <c r="Y85" s="14"/>
       <c r="Z85" s="14"/>
       <c r="AA85" s="14"/>
     </row>
     <row r="86" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B86" s="40" t="s">
+      <c r="B86" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="41"/>
-      <c r="D86" s="41"/>
-      <c r="E86" s="41"/>
-      <c r="F86" s="41"/>
-      <c r="G86" s="42"/>
-      <c r="K86" s="40" t="s">
+      <c r="C86" s="47"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="47"/>
+      <c r="F86" s="47"/>
+      <c r="G86" s="48"/>
+      <c r="K86" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L86" s="41"/>
-      <c r="M86" s="41"/>
-      <c r="N86" s="41"/>
-      <c r="O86" s="41"/>
-      <c r="P86" s="42"/>
+      <c r="L86" s="47"/>
+      <c r="M86" s="47"/>
+      <c r="N86" s="47"/>
+      <c r="O86" s="47"/>
+      <c r="P86" s="48"/>
       <c r="X86" s="14"/>
       <c r="Y86" s="14"/>
       <c r="Z86" s="14"/>
       <c r="AA86" s="14"/>
     </row>
     <row r="87" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B87" s="40" t="s">
+      <c r="B87" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C87" s="41"/>
-      <c r="D87" s="41"/>
-      <c r="E87" s="41"/>
-      <c r="F87" s="41"/>
-      <c r="G87" s="42"/>
-      <c r="K87" s="40" t="s">
+      <c r="C87" s="47"/>
+      <c r="D87" s="47"/>
+      <c r="E87" s="47"/>
+      <c r="F87" s="47"/>
+      <c r="G87" s="48"/>
+      <c r="K87" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L87" s="41"/>
-      <c r="M87" s="41"/>
-      <c r="N87" s="41"/>
-      <c r="O87" s="41"/>
-      <c r="P87" s="42"/>
+      <c r="L87" s="47"/>
+      <c r="M87" s="47"/>
+      <c r="N87" s="47"/>
+      <c r="O87" s="47"/>
+      <c r="P87" s="48"/>
       <c r="X87" s="14"/>
       <c r="Y87" s="14"/>
       <c r="Z87" s="14"/>
       <c r="AA87" s="14"/>
     </row>
     <row r="88" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B88" s="40" t="s">
+      <c r="B88" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C88" s="41"/>
-      <c r="D88" s="41"/>
-      <c r="E88" s="41"/>
-      <c r="F88" s="41"/>
-      <c r="G88" s="42"/>
-      <c r="K88" s="40" t="s">
+      <c r="C88" s="47"/>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="48"/>
+      <c r="K88" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L88" s="41"/>
-      <c r="M88" s="41"/>
-      <c r="N88" s="41"/>
-      <c r="O88" s="41"/>
-      <c r="P88" s="42"/>
+      <c r="L88" s="47"/>
+      <c r="M88" s="47"/>
+      <c r="N88" s="47"/>
+      <c r="O88" s="47"/>
+      <c r="P88" s="48"/>
       <c r="X88" s="14"/>
       <c r="Y88" s="14"/>
       <c r="Z88" s="14"/>
       <c r="AA88" s="14"/>
     </row>
     <row r="89" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B89" s="40" t="s">
+      <c r="B89" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C89" s="41"/>
-      <c r="D89" s="41"/>
-      <c r="E89" s="41"/>
-      <c r="F89" s="41"/>
-      <c r="G89" s="42"/>
-      <c r="K89" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="L89" s="41"/>
-      <c r="M89" s="41"/>
-      <c r="N89" s="41"/>
-      <c r="O89" s="41"/>
-      <c r="P89" s="42"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="48"/>
+      <c r="K89" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="L89" s="47"/>
+      <c r="M89" s="47"/>
+      <c r="N89" s="47"/>
+      <c r="O89" s="47"/>
+      <c r="P89" s="48"/>
       <c r="X89" s="14"/>
       <c r="Y89" s="14"/>
       <c r="Z89" s="14"/>
       <c r="AA89" s="14"/>
     </row>
     <row r="90" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B90" s="40"/>
-      <c r="C90" s="41"/>
-      <c r="D90" s="41"/>
-      <c r="E90" s="41"/>
-      <c r="F90" s="41"/>
-      <c r="G90" s="42"/>
-      <c r="K90" s="40"/>
-      <c r="L90" s="41"/>
-      <c r="M90" s="41"/>
-      <c r="N90" s="41"/>
-      <c r="O90" s="41"/>
-      <c r="P90" s="42"/>
+      <c r="B90" s="46"/>
+      <c r="C90" s="47"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="47"/>
+      <c r="G90" s="48"/>
+      <c r="K90" s="46"/>
+      <c r="L90" s="47"/>
+      <c r="M90" s="47"/>
+      <c r="N90" s="47"/>
+      <c r="O90" s="47"/>
+      <c r="P90" s="48"/>
       <c r="X90" s="14"/>
       <c r="Y90" s="14"/>
       <c r="Z90" s="14"/>
       <c r="AA90" s="14"/>
     </row>
     <row r="91" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B91" s="40" t="s">
+      <c r="B91" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41"/>
-      <c r="E91" s="41"/>
-      <c r="F91" s="41"/>
-      <c r="G91" s="42"/>
-      <c r="K91" s="40" t="s">
+      <c r="C91" s="47"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="47"/>
+      <c r="F91" s="47"/>
+      <c r="G91" s="48"/>
+      <c r="K91" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L91" s="41"/>
-      <c r="M91" s="41"/>
-      <c r="N91" s="41"/>
-      <c r="O91" s="41"/>
-      <c r="P91" s="42"/>
+      <c r="L91" s="47"/>
+      <c r="M91" s="47"/>
+      <c r="N91" s="47"/>
+      <c r="O91" s="47"/>
+      <c r="P91" s="48"/>
       <c r="X91" s="14"/>
       <c r="Y91" s="14"/>
       <c r="Z91" s="14"/>
       <c r="AA91" s="14"/>
     </row>
     <row r="92" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B92" s="40" t="s">
+      <c r="B92" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="C92" s="41"/>
-      <c r="D92" s="41"/>
-      <c r="E92" s="41"/>
-      <c r="F92" s="41"/>
-      <c r="G92" s="42"/>
-      <c r="K92" s="40" t="s">
+      <c r="C92" s="47"/>
+      <c r="D92" s="47"/>
+      <c r="E92" s="47"/>
+      <c r="F92" s="47"/>
+      <c r="G92" s="48"/>
+      <c r="K92" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="L92" s="41"/>
-      <c r="M92" s="41"/>
-      <c r="N92" s="41"/>
-      <c r="O92" s="41"/>
-      <c r="P92" s="42"/>
+      <c r="L92" s="47"/>
+      <c r="M92" s="47"/>
+      <c r="N92" s="47"/>
+      <c r="O92" s="47"/>
+      <c r="P92" s="48"/>
       <c r="X92" s="14"/>
       <c r="Y92" s="14"/>
       <c r="Z92" s="14"/>
       <c r="AA92" s="14"/>
     </row>
     <row r="93" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B93" s="40"/>
-      <c r="C93" s="41"/>
-      <c r="D93" s="41"/>
-      <c r="E93" s="41"/>
-      <c r="F93" s="41"/>
-      <c r="G93" s="42"/>
-      <c r="K93" s="40"/>
-      <c r="L93" s="41"/>
-      <c r="M93" s="41"/>
-      <c r="N93" s="41"/>
-      <c r="O93" s="41"/>
-      <c r="P93" s="42"/>
+      <c r="B93" s="46"/>
+      <c r="C93" s="47"/>
+      <c r="D93" s="47"/>
+      <c r="E93" s="47"/>
+      <c r="F93" s="47"/>
+      <c r="G93" s="48"/>
+      <c r="K93" s="46"/>
+      <c r="L93" s="47"/>
+      <c r="M93" s="47"/>
+      <c r="N93" s="47"/>
+      <c r="O93" s="47"/>
+      <c r="P93" s="48"/>
       <c r="X93" s="14"/>
       <c r="Y93" s="14"/>
       <c r="Z93" s="14"/>
       <c r="AA93" s="14"/>
     </row>
     <row r="94" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B94" s="40"/>
-      <c r="C94" s="41"/>
-      <c r="D94" s="41"/>
-      <c r="E94" s="41"/>
-      <c r="F94" s="41"/>
-      <c r="G94" s="42"/>
-      <c r="K94" s="40"/>
-      <c r="L94" s="41"/>
-      <c r="M94" s="41"/>
-      <c r="N94" s="41"/>
-      <c r="O94" s="41"/>
-      <c r="P94" s="42"/>
+      <c r="B94" s="46"/>
+      <c r="C94" s="47"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="48"/>
+      <c r="K94" s="46"/>
+      <c r="L94" s="47"/>
+      <c r="M94" s="47"/>
+      <c r="N94" s="47"/>
+      <c r="O94" s="47"/>
+      <c r="P94" s="48"/>
       <c r="X94" s="14"/>
       <c r="Y94" s="14"/>
       <c r="Z94" s="14"/>
       <c r="AA94" s="14"/>
     </row>
     <row r="95" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B95" s="48" t="s">
+      <c r="B95" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C95" s="49"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="49"/>
-      <c r="F95" s="49"/>
-      <c r="G95" s="50"/>
-      <c r="K95" s="40" t="s">
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="45"/>
+      <c r="K95" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="L95" s="41"/>
-      <c r="M95" s="41"/>
-      <c r="N95" s="41"/>
-      <c r="O95" s="41"/>
-      <c r="P95" s="42"/>
+      <c r="L95" s="47"/>
+      <c r="M95" s="47"/>
+      <c r="N95" s="47"/>
+      <c r="O95" s="47"/>
+      <c r="P95" s="48"/>
       <c r="X95" s="14"/>
       <c r="Y95" s="14"/>
       <c r="Z95" s="14"/>
@@ -2772,14 +2775,14 @@
       <c r="E96" s="38"/>
       <c r="F96" s="38"/>
       <c r="G96" s="39"/>
-      <c r="K96" s="40" t="s">
+      <c r="K96" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="L96" s="41"/>
-      <c r="M96" s="41"/>
-      <c r="N96" s="41"/>
-      <c r="O96" s="41"/>
-      <c r="P96" s="42"/>
+      <c r="L96" s="47"/>
+      <c r="M96" s="47"/>
+      <c r="N96" s="47"/>
+      <c r="O96" s="47"/>
+      <c r="P96" s="48"/>
       <c r="X96" s="14"/>
       <c r="Y96" s="14"/>
       <c r="Z96" s="14"/>
@@ -2794,14 +2797,14 @@
       <c r="E97" s="38"/>
       <c r="F97" s="38"/>
       <c r="G97" s="39"/>
-      <c r="K97" s="40" t="s">
+      <c r="K97" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="L97" s="41"/>
-      <c r="M97" s="41"/>
-      <c r="N97" s="41"/>
-      <c r="O97" s="41"/>
-      <c r="P97" s="42"/>
+      <c r="L97" s="47"/>
+      <c r="M97" s="47"/>
+      <c r="N97" s="47"/>
+      <c r="O97" s="47"/>
+      <c r="P97" s="48"/>
       <c r="X97" s="14"/>
       <c r="Y97" s="14"/>
       <c r="Z97" s="14"/>
@@ -2816,14 +2819,14 @@
       <c r="E98" s="38"/>
       <c r="F98" s="38"/>
       <c r="G98" s="39"/>
-      <c r="K98" s="40" t="s">
+      <c r="K98" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="L98" s="41"/>
-      <c r="M98" s="41"/>
-      <c r="N98" s="41"/>
-      <c r="O98" s="41"/>
-      <c r="P98" s="42"/>
+      <c r="L98" s="47"/>
+      <c r="M98" s="47"/>
+      <c r="N98" s="47"/>
+      <c r="O98" s="47"/>
+      <c r="P98" s="48"/>
       <c r="X98" s="14"/>
       <c r="Y98" s="14"/>
       <c r="Z98" s="14"/>
@@ -2838,14 +2841,14 @@
       <c r="E99" s="38"/>
       <c r="F99" s="38"/>
       <c r="G99" s="39"/>
-      <c r="K99" s="40" t="s">
+      <c r="K99" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="L99" s="41"/>
-      <c r="M99" s="41"/>
-      <c r="N99" s="41"/>
-      <c r="O99" s="41"/>
-      <c r="P99" s="42"/>
+      <c r="L99" s="47"/>
+      <c r="M99" s="47"/>
+      <c r="N99" s="47"/>
+      <c r="O99" s="47"/>
+      <c r="P99" s="48"/>
       <c r="X99" s="14"/>
       <c r="Y99" s="14"/>
       <c r="Z99" s="14"/>
@@ -2858,12 +2861,12 @@
       <c r="E100" s="38"/>
       <c r="F100" s="38"/>
       <c r="G100" s="39"/>
-      <c r="K100" s="40"/>
-      <c r="L100" s="41"/>
-      <c r="M100" s="41"/>
-      <c r="N100" s="41"/>
-      <c r="O100" s="41"/>
-      <c r="P100" s="42"/>
+      <c r="K100" s="46"/>
+      <c r="L100" s="47"/>
+      <c r="M100" s="47"/>
+      <c r="N100" s="47"/>
+      <c r="O100" s="47"/>
+      <c r="P100" s="48"/>
       <c r="X100" s="14"/>
       <c r="Y100" s="14"/>
       <c r="Z100" s="14"/>
@@ -2878,14 +2881,14 @@
       <c r="E101" s="38"/>
       <c r="F101" s="38"/>
       <c r="G101" s="39"/>
-      <c r="K101" s="40" t="s">
+      <c r="K101" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="L101" s="41"/>
-      <c r="M101" s="41"/>
-      <c r="N101" s="41"/>
-      <c r="O101" s="41"/>
-      <c r="P101" s="42"/>
+      <c r="L101" s="47"/>
+      <c r="M101" s="47"/>
+      <c r="N101" s="47"/>
+      <c r="O101" s="47"/>
+      <c r="P101" s="48"/>
       <c r="X101" s="14"/>
       <c r="Y101" s="14"/>
       <c r="Z101" s="14"/>
@@ -2898,12 +2901,12 @@
       <c r="E102" s="38"/>
       <c r="F102" s="38"/>
       <c r="G102" s="39"/>
-      <c r="K102" s="40"/>
-      <c r="L102" s="41"/>
-      <c r="M102" s="41"/>
-      <c r="N102" s="41"/>
-      <c r="O102" s="41"/>
-      <c r="P102" s="42"/>
+      <c r="K102" s="46"/>
+      <c r="L102" s="47"/>
+      <c r="M102" s="47"/>
+      <c r="N102" s="47"/>
+      <c r="O102" s="47"/>
+      <c r="P102" s="48"/>
       <c r="X102" s="14"/>
       <c r="Y102" s="14"/>
       <c r="Z102" s="14"/>
@@ -2916,34 +2919,34 @@
       <c r="E103" s="38"/>
       <c r="F103" s="38"/>
       <c r="G103" s="39"/>
-      <c r="K103" s="40"/>
-      <c r="L103" s="41"/>
-      <c r="M103" s="41"/>
-      <c r="N103" s="41"/>
-      <c r="O103" s="41"/>
-      <c r="P103" s="42"/>
+      <c r="K103" s="46"/>
+      <c r="L103" s="47"/>
+      <c r="M103" s="47"/>
+      <c r="N103" s="47"/>
+      <c r="O103" s="47"/>
+      <c r="P103" s="48"/>
       <c r="X103" s="14"/>
       <c r="Y103" s="14"/>
       <c r="Z103" s="14"/>
       <c r="AA103" s="14"/>
     </row>
     <row r="104" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B104" s="48" t="s">
+      <c r="B104" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C104" s="49"/>
-      <c r="D104" s="49"/>
-      <c r="E104" s="49"/>
-      <c r="F104" s="49"/>
-      <c r="G104" s="50"/>
-      <c r="K104" s="40" t="s">
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="45"/>
+      <c r="K104" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L104" s="41"/>
-      <c r="M104" s="41"/>
-      <c r="N104" s="41"/>
-      <c r="O104" s="41"/>
-      <c r="P104" s="42"/>
+      <c r="L104" s="47"/>
+      <c r="M104" s="47"/>
+      <c r="N104" s="47"/>
+      <c r="O104" s="47"/>
+      <c r="P104" s="48"/>
       <c r="X104" s="14"/>
       <c r="Y104" s="14"/>
       <c r="Z104" s="14"/>
@@ -2958,14 +2961,14 @@
       <c r="E105" s="38"/>
       <c r="F105" s="38"/>
       <c r="G105" s="39"/>
-      <c r="K105" s="40" t="s">
+      <c r="K105" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="L105" s="41"/>
-      <c r="M105" s="41"/>
-      <c r="N105" s="41"/>
-      <c r="O105" s="41"/>
-      <c r="P105" s="42"/>
+      <c r="L105" s="47"/>
+      <c r="M105" s="47"/>
+      <c r="N105" s="47"/>
+      <c r="O105" s="47"/>
+      <c r="P105" s="48"/>
       <c r="X105" s="14"/>
       <c r="Y105" s="14"/>
       <c r="Z105" s="14"/>
@@ -2980,14 +2983,14 @@
       <c r="E106" s="38"/>
       <c r="F106" s="38"/>
       <c r="G106" s="39"/>
-      <c r="K106" s="40" t="s">
+      <c r="K106" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="L106" s="41"/>
-      <c r="M106" s="41"/>
-      <c r="N106" s="41"/>
-      <c r="O106" s="41"/>
-      <c r="P106" s="42"/>
+      <c r="L106" s="47"/>
+      <c r="M106" s="47"/>
+      <c r="N106" s="47"/>
+      <c r="O106" s="47"/>
+      <c r="P106" s="48"/>
       <c r="X106" s="14"/>
       <c r="Y106" s="14"/>
       <c r="Z106" s="14"/>
@@ -3000,52 +3003,52 @@
       <c r="E107" s="38"/>
       <c r="F107" s="38"/>
       <c r="G107" s="39"/>
-      <c r="K107" s="40"/>
-      <c r="L107" s="41"/>
-      <c r="M107" s="41"/>
-      <c r="N107" s="41"/>
-      <c r="O107" s="41"/>
-      <c r="P107" s="42"/>
+      <c r="K107" s="46"/>
+      <c r="L107" s="47"/>
+      <c r="M107" s="47"/>
+      <c r="N107" s="47"/>
+      <c r="O107" s="47"/>
+      <c r="P107" s="48"/>
       <c r="X107" s="14"/>
       <c r="Y107" s="14"/>
       <c r="Z107" s="14"/>
       <c r="AA107" s="14"/>
     </row>
     <row r="108" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B108" s="51"/>
-      <c r="C108" s="52"/>
-      <c r="D108" s="52"/>
-      <c r="E108" s="52"/>
-      <c r="F108" s="52"/>
-      <c r="G108" s="53"/>
-      <c r="K108" s="40"/>
-      <c r="L108" s="41"/>
-      <c r="M108" s="41"/>
-      <c r="N108" s="41"/>
-      <c r="O108" s="41"/>
-      <c r="P108" s="42"/>
+      <c r="B108" s="40"/>
+      <c r="C108" s="41"/>
+      <c r="D108" s="41"/>
+      <c r="E108" s="41"/>
+      <c r="F108" s="41"/>
+      <c r="G108" s="42"/>
+      <c r="K108" s="46"/>
+      <c r="L108" s="47"/>
+      <c r="M108" s="47"/>
+      <c r="N108" s="47"/>
+      <c r="O108" s="47"/>
+      <c r="P108" s="48"/>
       <c r="X108" s="14"/>
       <c r="Y108" s="14"/>
       <c r="Z108" s="14"/>
       <c r="AA108" s="14"/>
     </row>
     <row r="109" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B109" s="48" t="s">
+      <c r="B109" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="C109" s="49"/>
-      <c r="D109" s="49"/>
-      <c r="E109" s="49"/>
-      <c r="F109" s="49"/>
-      <c r="G109" s="50"/>
-      <c r="K109" s="40" t="s">
+      <c r="C109" s="44"/>
+      <c r="D109" s="44"/>
+      <c r="E109" s="44"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="45"/>
+      <c r="K109" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="L109" s="41"/>
-      <c r="M109" s="41"/>
-      <c r="N109" s="41"/>
-      <c r="O109" s="41"/>
-      <c r="P109" s="42"/>
+      <c r="L109" s="47"/>
+      <c r="M109" s="47"/>
+      <c r="N109" s="47"/>
+      <c r="O109" s="47"/>
+      <c r="P109" s="48"/>
       <c r="X109" s="14"/>
       <c r="Y109" s="14"/>
       <c r="Z109" s="14"/>
@@ -3060,14 +3063,14 @@
       <c r="E110" s="38"/>
       <c r="F110" s="38"/>
       <c r="G110" s="39"/>
-      <c r="K110" s="40" t="s">
+      <c r="K110" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="L110" s="41"/>
-      <c r="M110" s="41"/>
-      <c r="N110" s="41"/>
-      <c r="O110" s="41"/>
-      <c r="P110" s="42"/>
+      <c r="L110" s="47"/>
+      <c r="M110" s="47"/>
+      <c r="N110" s="47"/>
+      <c r="O110" s="47"/>
+      <c r="P110" s="48"/>
       <c r="X110" s="14"/>
       <c r="Y110" s="14"/>
       <c r="Z110" s="14"/>
@@ -3082,14 +3085,14 @@
       <c r="E111" s="38"/>
       <c r="F111" s="38"/>
       <c r="G111" s="39"/>
-      <c r="K111" s="40" t="s">
+      <c r="K111" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L111" s="41"/>
-      <c r="M111" s="41"/>
-      <c r="N111" s="41"/>
-      <c r="O111" s="41"/>
-      <c r="P111" s="42"/>
+      <c r="L111" s="47"/>
+      <c r="M111" s="47"/>
+      <c r="N111" s="47"/>
+      <c r="O111" s="47"/>
+      <c r="P111" s="48"/>
       <c r="X111" s="14"/>
       <c r="Y111" s="14"/>
       <c r="Z111" s="14"/>
@@ -3104,14 +3107,14 @@
       <c r="E112" s="38"/>
       <c r="F112" s="38"/>
       <c r="G112" s="39"/>
-      <c r="K112" s="40" t="s">
+      <c r="K112" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="L112" s="41"/>
-      <c r="M112" s="41"/>
-      <c r="N112" s="41"/>
-      <c r="O112" s="41"/>
-      <c r="P112" s="42"/>
+      <c r="L112" s="47"/>
+      <c r="M112" s="47"/>
+      <c r="N112" s="47"/>
+      <c r="O112" s="47"/>
+      <c r="P112" s="48"/>
       <c r="X112" s="14"/>
       <c r="Y112" s="14"/>
       <c r="Z112" s="14"/>
@@ -3126,14 +3129,14 @@
       <c r="E113" s="38"/>
       <c r="F113" s="38"/>
       <c r="G113" s="39"/>
-      <c r="K113" s="40" t="s">
+      <c r="K113" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="L113" s="41"/>
-      <c r="M113" s="41"/>
-      <c r="N113" s="41"/>
-      <c r="O113" s="41"/>
-      <c r="P113" s="42"/>
+      <c r="L113" s="47"/>
+      <c r="M113" s="47"/>
+      <c r="N113" s="47"/>
+      <c r="O113" s="47"/>
+      <c r="P113" s="48"/>
       <c r="X113" s="14"/>
       <c r="Y113" s="14"/>
       <c r="Z113" s="14"/>
@@ -3148,14 +3151,14 @@
       <c r="E114" s="38"/>
       <c r="F114" s="38"/>
       <c r="G114" s="39"/>
-      <c r="K114" s="40" t="s">
+      <c r="K114" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="L114" s="41"/>
-      <c r="M114" s="41"/>
-      <c r="N114" s="41"/>
-      <c r="O114" s="41"/>
-      <c r="P114" s="42"/>
+      <c r="L114" s="47"/>
+      <c r="M114" s="47"/>
+      <c r="N114" s="47"/>
+      <c r="O114" s="47"/>
+      <c r="P114" s="48"/>
       <c r="X114" s="14"/>
       <c r="Y114" s="14"/>
       <c r="Z114" s="14"/>
@@ -3170,72 +3173,72 @@
       <c r="E115" s="38"/>
       <c r="F115" s="38"/>
       <c r="G115" s="39"/>
-      <c r="K115" s="40" t="s">
+      <c r="K115" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="L115" s="41"/>
-      <c r="M115" s="41"/>
-      <c r="N115" s="41"/>
-      <c r="O115" s="41"/>
-      <c r="P115" s="42"/>
+      <c r="L115" s="47"/>
+      <c r="M115" s="47"/>
+      <c r="N115" s="47"/>
+      <c r="O115" s="47"/>
+      <c r="P115" s="48"/>
       <c r="X115" s="14"/>
       <c r="Y115" s="14"/>
       <c r="Z115" s="14"/>
       <c r="AA115" s="14"/>
     </row>
     <row r="116" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B116" s="51"/>
-      <c r="C116" s="52"/>
-      <c r="D116" s="52"/>
-      <c r="E116" s="52"/>
-      <c r="F116" s="52"/>
-      <c r="G116" s="53"/>
-      <c r="K116" s="40"/>
-      <c r="L116" s="41"/>
-      <c r="M116" s="41"/>
-      <c r="N116" s="41"/>
-      <c r="O116" s="41"/>
-      <c r="P116" s="42"/>
+      <c r="B116" s="40"/>
+      <c r="C116" s="41"/>
+      <c r="D116" s="41"/>
+      <c r="E116" s="41"/>
+      <c r="F116" s="41"/>
+      <c r="G116" s="42"/>
+      <c r="K116" s="46"/>
+      <c r="L116" s="47"/>
+      <c r="M116" s="47"/>
+      <c r="N116" s="47"/>
+      <c r="O116" s="47"/>
+      <c r="P116" s="48"/>
       <c r="X116" s="14"/>
       <c r="Y116" s="14"/>
       <c r="Z116" s="14"/>
       <c r="AA116" s="14"/>
     </row>
     <row r="117" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B117" s="51"/>
-      <c r="C117" s="52"/>
-      <c r="D117" s="52"/>
-      <c r="E117" s="52"/>
-      <c r="F117" s="52"/>
-      <c r="G117" s="53"/>
-      <c r="K117" s="40"/>
-      <c r="L117" s="41"/>
-      <c r="M117" s="41"/>
-      <c r="N117" s="41"/>
-      <c r="O117" s="41"/>
-      <c r="P117" s="42"/>
+      <c r="B117" s="40"/>
+      <c r="C117" s="41"/>
+      <c r="D117" s="41"/>
+      <c r="E117" s="41"/>
+      <c r="F117" s="41"/>
+      <c r="G117" s="42"/>
+      <c r="K117" s="46"/>
+      <c r="L117" s="47"/>
+      <c r="M117" s="47"/>
+      <c r="N117" s="47"/>
+      <c r="O117" s="47"/>
+      <c r="P117" s="48"/>
       <c r="X117" s="14"/>
       <c r="Y117" s="14"/>
       <c r="Z117" s="14"/>
       <c r="AA117" s="14"/>
     </row>
     <row r="118" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B118" s="48" t="s">
+      <c r="B118" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C118" s="49"/>
-      <c r="D118" s="49"/>
-      <c r="E118" s="49"/>
-      <c r="F118" s="49"/>
-      <c r="G118" s="50"/>
-      <c r="K118" s="40" t="s">
+      <c r="C118" s="44"/>
+      <c r="D118" s="44"/>
+      <c r="E118" s="44"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="45"/>
+      <c r="K118" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L118" s="41"/>
-      <c r="M118" s="41"/>
-      <c r="N118" s="41"/>
-      <c r="O118" s="41"/>
-      <c r="P118" s="42"/>
+      <c r="L118" s="47"/>
+      <c r="M118" s="47"/>
+      <c r="N118" s="47"/>
+      <c r="O118" s="47"/>
+      <c r="P118" s="48"/>
       <c r="X118" s="13"/>
       <c r="Y118" s="13"/>
       <c r="Z118" s="13"/>
@@ -3245,19 +3248,19 @@
       <c r="B119" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="C119" s="52"/>
-      <c r="D119" s="52"/>
-      <c r="E119" s="52"/>
-      <c r="F119" s="52"/>
-      <c r="G119" s="53"/>
-      <c r="K119" s="40" t="s">
+      <c r="C119" s="41"/>
+      <c r="D119" s="41"/>
+      <c r="E119" s="41"/>
+      <c r="F119" s="41"/>
+      <c r="G119" s="42"/>
+      <c r="K119" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L119" s="41"/>
-      <c r="M119" s="41"/>
-      <c r="N119" s="41"/>
-      <c r="O119" s="41"/>
-      <c r="P119" s="42"/>
+      <c r="L119" s="47"/>
+      <c r="M119" s="47"/>
+      <c r="N119" s="47"/>
+      <c r="O119" s="47"/>
+      <c r="P119" s="48"/>
       <c r="X119" s="13"/>
       <c r="Y119" s="13"/>
       <c r="Z119" s="13"/>
@@ -3267,19 +3270,19 @@
       <c r="B120" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C120" s="52"/>
-      <c r="D120" s="52"/>
-      <c r="E120" s="52"/>
-      <c r="F120" s="52"/>
-      <c r="G120" s="53"/>
-      <c r="K120" s="40" t="s">
+      <c r="C120" s="41"/>
+      <c r="D120" s="41"/>
+      <c r="E120" s="41"/>
+      <c r="F120" s="41"/>
+      <c r="G120" s="42"/>
+      <c r="K120" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L120" s="41"/>
-      <c r="M120" s="41"/>
-      <c r="N120" s="41"/>
-      <c r="O120" s="41"/>
-      <c r="P120" s="42"/>
+      <c r="L120" s="47"/>
+      <c r="M120" s="47"/>
+      <c r="N120" s="47"/>
+      <c r="O120" s="47"/>
+      <c r="P120" s="48"/>
       <c r="X120" s="13"/>
       <c r="Y120" s="13"/>
       <c r="Z120" s="13"/>
@@ -3294,70 +3297,70 @@
       <c r="E121" s="38"/>
       <c r="F121" s="38"/>
       <c r="G121" s="39"/>
-      <c r="K121" s="40" t="s">
+      <c r="K121" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L121" s="41"/>
-      <c r="M121" s="41"/>
-      <c r="N121" s="41"/>
-      <c r="O121" s="41"/>
-      <c r="P121" s="42"/>
+      <c r="L121" s="47"/>
+      <c r="M121" s="47"/>
+      <c r="N121" s="47"/>
+      <c r="O121" s="47"/>
+      <c r="P121" s="48"/>
       <c r="X121" s="13"/>
       <c r="Y121" s="13"/>
       <c r="Z121" s="13"/>
       <c r="AA121" s="13"/>
     </row>
     <row r="122" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B122" s="40"/>
-      <c r="C122" s="41"/>
-      <c r="D122" s="41"/>
-      <c r="E122" s="41"/>
-      <c r="F122" s="41"/>
-      <c r="G122" s="42"/>
-      <c r="K122" s="40"/>
-      <c r="L122" s="41"/>
-      <c r="M122" s="41"/>
-      <c r="N122" s="41"/>
-      <c r="O122" s="41"/>
-      <c r="P122" s="42"/>
+      <c r="B122" s="46"/>
+      <c r="C122" s="47"/>
+      <c r="D122" s="47"/>
+      <c r="E122" s="47"/>
+      <c r="F122" s="47"/>
+      <c r="G122" s="48"/>
+      <c r="K122" s="46"/>
+      <c r="L122" s="47"/>
+      <c r="M122" s="47"/>
+      <c r="N122" s="47"/>
+      <c r="O122" s="47"/>
+      <c r="P122" s="48"/>
       <c r="X122" s="14"/>
       <c r="Y122" s="14"/>
       <c r="Z122" s="14"/>
       <c r="AA122" s="14"/>
     </row>
     <row r="123" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B123" s="40"/>
-      <c r="C123" s="41"/>
-      <c r="D123" s="41"/>
-      <c r="E123" s="41"/>
-      <c r="F123" s="41"/>
-      <c r="G123" s="42"/>
-      <c r="K123" s="40"/>
-      <c r="L123" s="41"/>
-      <c r="M123" s="41"/>
-      <c r="N123" s="41"/>
-      <c r="O123" s="41"/>
-      <c r="P123" s="42"/>
+      <c r="B123" s="46"/>
+      <c r="C123" s="47"/>
+      <c r="D123" s="47"/>
+      <c r="E123" s="47"/>
+      <c r="F123" s="47"/>
+      <c r="G123" s="48"/>
+      <c r="K123" s="46"/>
+      <c r="L123" s="47"/>
+      <c r="M123" s="47"/>
+      <c r="N123" s="47"/>
+      <c r="O123" s="47"/>
+      <c r="P123" s="48"/>
       <c r="X123" s="14"/>
       <c r="Y123" s="14"/>
       <c r="Z123" s="14"/>
       <c r="AA123" s="14"/>
     </row>
     <row r="124" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B124" s="48" t="s">
+      <c r="B124" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C124" s="49"/>
-      <c r="D124" s="49"/>
-      <c r="E124" s="49"/>
-      <c r="F124" s="49"/>
-      <c r="G124" s="50"/>
-      <c r="K124" s="40"/>
-      <c r="L124" s="41"/>
-      <c r="M124" s="41"/>
-      <c r="N124" s="41"/>
-      <c r="O124" s="41"/>
-      <c r="P124" s="42"/>
+      <c r="C124" s="44"/>
+      <c r="D124" s="44"/>
+      <c r="E124" s="44"/>
+      <c r="F124" s="44"/>
+      <c r="G124" s="45"/>
+      <c r="K124" s="46"/>
+      <c r="L124" s="47"/>
+      <c r="M124" s="47"/>
+      <c r="N124" s="47"/>
+      <c r="O124" s="47"/>
+      <c r="P124" s="48"/>
       <c r="X124" s="14"/>
       <c r="Y124" s="14"/>
       <c r="Z124" s="14"/>
@@ -3372,14 +3375,14 @@
       <c r="E125" s="38"/>
       <c r="F125" s="38"/>
       <c r="G125" s="39"/>
-      <c r="K125" s="40" t="s">
+      <c r="K125" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="L125" s="41"/>
-      <c r="M125" s="41"/>
-      <c r="N125" s="41"/>
-      <c r="O125" s="41"/>
-      <c r="P125" s="42"/>
+      <c r="L125" s="47"/>
+      <c r="M125" s="47"/>
+      <c r="N125" s="47"/>
+      <c r="O125" s="47"/>
+      <c r="P125" s="48"/>
       <c r="X125" s="14"/>
       <c r="Y125" s="14"/>
       <c r="Z125" s="14"/>
@@ -3394,14 +3397,14 @@
       <c r="E126" s="38"/>
       <c r="F126" s="38"/>
       <c r="G126" s="39"/>
-      <c r="K126" s="40" t="s">
+      <c r="K126" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="L126" s="41"/>
-      <c r="M126" s="41"/>
-      <c r="N126" s="41"/>
-      <c r="O126" s="41"/>
-      <c r="P126" s="42"/>
+      <c r="L126" s="47"/>
+      <c r="M126" s="47"/>
+      <c r="N126" s="47"/>
+      <c r="O126" s="47"/>
+      <c r="P126" s="48"/>
       <c r="X126" s="14"/>
       <c r="Y126" s="14"/>
       <c r="Z126" s="14"/>
@@ -3416,14 +3419,14 @@
       <c r="E127" s="38"/>
       <c r="F127" s="38"/>
       <c r="G127" s="39"/>
-      <c r="K127" s="40" t="s">
+      <c r="K127" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="L127" s="41"/>
-      <c r="M127" s="41"/>
-      <c r="N127" s="41"/>
-      <c r="O127" s="41"/>
-      <c r="P127" s="42"/>
+      <c r="L127" s="47"/>
+      <c r="M127" s="47"/>
+      <c r="N127" s="47"/>
+      <c r="O127" s="47"/>
+      <c r="P127" s="48"/>
       <c r="X127" s="14"/>
       <c r="Y127" s="14"/>
       <c r="Z127" s="14"/>
@@ -3438,14 +3441,14 @@
       <c r="E128" s="38"/>
       <c r="F128" s="38"/>
       <c r="G128" s="39"/>
-      <c r="K128" s="40" t="s">
+      <c r="K128" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L128" s="41"/>
-      <c r="M128" s="41"/>
-      <c r="N128" s="41"/>
-      <c r="O128" s="41"/>
-      <c r="P128" s="42"/>
+      <c r="L128" s="47"/>
+      <c r="M128" s="47"/>
+      <c r="N128" s="47"/>
+      <c r="O128" s="47"/>
+      <c r="P128" s="48"/>
       <c r="X128" s="14"/>
       <c r="Y128" s="14"/>
       <c r="Z128" s="14"/>
@@ -3460,14 +3463,14 @@
       <c r="E129" s="38"/>
       <c r="F129" s="38"/>
       <c r="G129" s="39"/>
-      <c r="K129" s="40" t="s">
+      <c r="K129" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="L129" s="41"/>
-      <c r="M129" s="41"/>
-      <c r="N129" s="41"/>
-      <c r="O129" s="41"/>
-      <c r="P129" s="42"/>
+      <c r="L129" s="47"/>
+      <c r="M129" s="47"/>
+      <c r="N129" s="47"/>
+      <c r="O129" s="47"/>
+      <c r="P129" s="48"/>
       <c r="X129" s="14"/>
       <c r="Y129" s="14"/>
       <c r="Z129" s="14"/>
@@ -3482,14 +3485,14 @@
       <c r="E130" s="38"/>
       <c r="F130" s="38"/>
       <c r="G130" s="39"/>
-      <c r="K130" s="40" t="s">
+      <c r="K130" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="L130" s="41"/>
-      <c r="M130" s="41"/>
-      <c r="N130" s="41"/>
-      <c r="O130" s="41"/>
-      <c r="P130" s="42"/>
+      <c r="L130" s="47"/>
+      <c r="M130" s="47"/>
+      <c r="N130" s="47"/>
+      <c r="O130" s="47"/>
+      <c r="P130" s="48"/>
       <c r="X130" s="14"/>
       <c r="Y130" s="14"/>
       <c r="Z130" s="14"/>
@@ -3504,14 +3507,14 @@
       <c r="E131" s="38"/>
       <c r="F131" s="38"/>
       <c r="G131" s="39"/>
-      <c r="K131" s="40" t="s">
+      <c r="K131" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="L131" s="41"/>
-      <c r="M131" s="41"/>
-      <c r="N131" s="41"/>
-      <c r="O131" s="41"/>
-      <c r="P131" s="42"/>
+      <c r="L131" s="47"/>
+      <c r="M131" s="47"/>
+      <c r="N131" s="47"/>
+      <c r="O131" s="47"/>
+      <c r="P131" s="48"/>
       <c r="X131" s="14"/>
       <c r="Y131" s="14"/>
       <c r="Z131" s="14"/>
@@ -3526,14 +3529,14 @@
       <c r="E132" s="38"/>
       <c r="F132" s="38"/>
       <c r="G132" s="39"/>
-      <c r="K132" s="40" t="s">
+      <c r="K132" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="L132" s="41"/>
-      <c r="M132" s="41"/>
-      <c r="N132" s="41"/>
-      <c r="O132" s="41"/>
-      <c r="P132" s="42"/>
+      <c r="L132" s="47"/>
+      <c r="M132" s="47"/>
+      <c r="N132" s="47"/>
+      <c r="O132" s="47"/>
+      <c r="P132" s="48"/>
       <c r="X132" s="14"/>
       <c r="Y132" s="14"/>
       <c r="Z132" s="14"/>
@@ -3548,256 +3551,256 @@
       <c r="E133" s="38"/>
       <c r="F133" s="38"/>
       <c r="G133" s="39"/>
-      <c r="K133" s="40" t="s">
+      <c r="K133" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="L133" s="41"/>
-      <c r="M133" s="41"/>
-      <c r="N133" s="41"/>
-      <c r="O133" s="41"/>
-      <c r="P133" s="42"/>
+      <c r="L133" s="47"/>
+      <c r="M133" s="47"/>
+      <c r="N133" s="47"/>
+      <c r="O133" s="47"/>
+      <c r="P133" s="48"/>
       <c r="X133" s="14"/>
       <c r="Y133" s="14"/>
       <c r="Z133" s="14"/>
       <c r="AA133" s="14"/>
     </row>
     <row r="134" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B134" s="51"/>
-      <c r="C134" s="52"/>
-      <c r="D134" s="52"/>
-      <c r="E134" s="52"/>
-      <c r="F134" s="52"/>
-      <c r="G134" s="53"/>
-      <c r="K134" s="40"/>
-      <c r="L134" s="41"/>
-      <c r="M134" s="41"/>
-      <c r="N134" s="41"/>
-      <c r="O134" s="41"/>
-      <c r="P134" s="42"/>
+      <c r="B134" s="40"/>
+      <c r="C134" s="41"/>
+      <c r="D134" s="41"/>
+      <c r="E134" s="41"/>
+      <c r="F134" s="41"/>
+      <c r="G134" s="42"/>
+      <c r="K134" s="46"/>
+      <c r="L134" s="47"/>
+      <c r="M134" s="47"/>
+      <c r="N134" s="47"/>
+      <c r="O134" s="47"/>
+      <c r="P134" s="48"/>
       <c r="X134" s="14"/>
       <c r="Y134" s="14"/>
       <c r="Z134" s="14"/>
       <c r="AA134" s="14"/>
     </row>
     <row r="135" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B135" s="51"/>
-      <c r="C135" s="52"/>
-      <c r="D135" s="52"/>
-      <c r="E135" s="52"/>
-      <c r="F135" s="52"/>
-      <c r="G135" s="53"/>
-      <c r="K135" s="40"/>
-      <c r="L135" s="41"/>
-      <c r="M135" s="41"/>
-      <c r="N135" s="41"/>
-      <c r="O135" s="41"/>
-      <c r="P135" s="42"/>
+      <c r="B135" s="40"/>
+      <c r="C135" s="41"/>
+      <c r="D135" s="41"/>
+      <c r="E135" s="41"/>
+      <c r="F135" s="41"/>
+      <c r="G135" s="42"/>
+      <c r="K135" s="46"/>
+      <c r="L135" s="47"/>
+      <c r="M135" s="47"/>
+      <c r="N135" s="47"/>
+      <c r="O135" s="47"/>
+      <c r="P135" s="48"/>
       <c r="X135" s="14"/>
       <c r="Y135" s="14"/>
       <c r="Z135" s="14"/>
       <c r="AA135" s="14"/>
     </row>
     <row r="136" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B136" s="51"/>
-      <c r="C136" s="52"/>
-      <c r="D136" s="52"/>
-      <c r="E136" s="52"/>
-      <c r="F136" s="52"/>
-      <c r="G136" s="53"/>
-      <c r="K136" s="40"/>
-      <c r="L136" s="41"/>
-      <c r="M136" s="41"/>
-      <c r="N136" s="41"/>
-      <c r="O136" s="41"/>
-      <c r="P136" s="42"/>
+      <c r="B136" s="40"/>
+      <c r="C136" s="41"/>
+      <c r="D136" s="41"/>
+      <c r="E136" s="41"/>
+      <c r="F136" s="41"/>
+      <c r="G136" s="42"/>
+      <c r="K136" s="46"/>
+      <c r="L136" s="47"/>
+      <c r="M136" s="47"/>
+      <c r="N136" s="47"/>
+      <c r="O136" s="47"/>
+      <c r="P136" s="48"/>
       <c r="X136" s="14"/>
       <c r="Y136" s="14"/>
       <c r="Z136" s="14"/>
       <c r="AA136" s="14"/>
     </row>
     <row r="137" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B137" s="40" t="s">
+      <c r="B137" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C137" s="41"/>
-      <c r="D137" s="41"/>
-      <c r="E137" s="41"/>
-      <c r="F137" s="41"/>
-      <c r="G137" s="42"/>
-      <c r="K137" s="40" t="s">
+      <c r="C137" s="47"/>
+      <c r="D137" s="47"/>
+      <c r="E137" s="47"/>
+      <c r="F137" s="47"/>
+      <c r="G137" s="48"/>
+      <c r="K137" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="L137" s="41"/>
-      <c r="M137" s="41"/>
-      <c r="N137" s="41"/>
-      <c r="O137" s="41"/>
-      <c r="P137" s="42"/>
+      <c r="L137" s="47"/>
+      <c r="M137" s="47"/>
+      <c r="N137" s="47"/>
+      <c r="O137" s="47"/>
+      <c r="P137" s="48"/>
       <c r="X137" s="13"/>
       <c r="Y137" s="13"/>
       <c r="Z137" s="13"/>
       <c r="AA137" s="13"/>
     </row>
     <row r="138" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B138" s="40" t="s">
+      <c r="B138" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C138" s="41"/>
-      <c r="D138" s="41"/>
-      <c r="E138" s="41"/>
-      <c r="F138" s="41"/>
-      <c r="G138" s="42"/>
-      <c r="K138" s="40" t="s">
+      <c r="C138" s="47"/>
+      <c r="D138" s="47"/>
+      <c r="E138" s="47"/>
+      <c r="F138" s="47"/>
+      <c r="G138" s="48"/>
+      <c r="K138" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="L138" s="41"/>
-      <c r="M138" s="41"/>
-      <c r="N138" s="41"/>
-      <c r="O138" s="41"/>
-      <c r="P138" s="42"/>
+      <c r="L138" s="47"/>
+      <c r="M138" s="47"/>
+      <c r="N138" s="47"/>
+      <c r="O138" s="47"/>
+      <c r="P138" s="48"/>
       <c r="X138" s="13"/>
       <c r="Y138" s="13"/>
       <c r="Z138" s="13"/>
       <c r="AA138" s="13"/>
     </row>
     <row r="139" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B139" s="40"/>
-      <c r="C139" s="41"/>
-      <c r="D139" s="41"/>
-      <c r="E139" s="41"/>
-      <c r="F139" s="41"/>
-      <c r="G139" s="42"/>
-      <c r="K139" s="40"/>
-      <c r="L139" s="41"/>
-      <c r="M139" s="41"/>
-      <c r="N139" s="41"/>
-      <c r="O139" s="41"/>
-      <c r="P139" s="42"/>
+      <c r="B139" s="46"/>
+      <c r="C139" s="47"/>
+      <c r="D139" s="47"/>
+      <c r="E139" s="47"/>
+      <c r="F139" s="47"/>
+      <c r="G139" s="48"/>
+      <c r="K139" s="46"/>
+      <c r="L139" s="47"/>
+      <c r="M139" s="47"/>
+      <c r="N139" s="47"/>
+      <c r="O139" s="47"/>
+      <c r="P139" s="48"/>
       <c r="X139" s="13"/>
       <c r="Y139" s="13"/>
       <c r="Z139" s="13"/>
       <c r="AA139" s="13"/>
     </row>
     <row r="140" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B140" s="40"/>
-      <c r="C140" s="41"/>
-      <c r="D140" s="41"/>
-      <c r="E140" s="41"/>
-      <c r="F140" s="41"/>
-      <c r="G140" s="42"/>
-      <c r="K140" s="40"/>
-      <c r="L140" s="41"/>
-      <c r="M140" s="41"/>
-      <c r="N140" s="41"/>
-      <c r="O140" s="41"/>
-      <c r="P140" s="42"/>
+      <c r="B140" s="46"/>
+      <c r="C140" s="47"/>
+      <c r="D140" s="47"/>
+      <c r="E140" s="47"/>
+      <c r="F140" s="47"/>
+      <c r="G140" s="48"/>
+      <c r="K140" s="46"/>
+      <c r="L140" s="47"/>
+      <c r="M140" s="47"/>
+      <c r="N140" s="47"/>
+      <c r="O140" s="47"/>
+      <c r="P140" s="48"/>
       <c r="X140" s="13"/>
       <c r="Y140" s="13"/>
       <c r="Z140" s="13"/>
       <c r="AA140" s="13"/>
     </row>
     <row r="141" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B141" s="48" t="s">
+      <c r="B141" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="C141" s="49"/>
-      <c r="D141" s="49"/>
-      <c r="E141" s="49"/>
-      <c r="F141" s="49"/>
-      <c r="G141" s="50"/>
-      <c r="K141" s="40"/>
-      <c r="L141" s="41"/>
-      <c r="M141" s="41"/>
-      <c r="N141" s="41"/>
-      <c r="O141" s="41"/>
-      <c r="P141" s="42"/>
+      <c r="C141" s="44"/>
+      <c r="D141" s="44"/>
+      <c r="E141" s="44"/>
+      <c r="F141" s="44"/>
+      <c r="G141" s="45"/>
+      <c r="K141" s="46"/>
+      <c r="L141" s="47"/>
+      <c r="M141" s="47"/>
+      <c r="N141" s="47"/>
+      <c r="O141" s="47"/>
+      <c r="P141" s="48"/>
       <c r="X141" s="13"/>
       <c r="Y141" s="13"/>
       <c r="Z141" s="13"/>
       <c r="AA141" s="13"/>
     </row>
     <row r="142" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B142" s="40" t="s">
+      <c r="B142" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C142" s="41"/>
-      <c r="D142" s="41"/>
-      <c r="E142" s="41"/>
-      <c r="F142" s="41"/>
-      <c r="G142" s="42"/>
-      <c r="K142" s="40" t="s">
+      <c r="C142" s="47"/>
+      <c r="D142" s="47"/>
+      <c r="E142" s="47"/>
+      <c r="F142" s="47"/>
+      <c r="G142" s="48"/>
+      <c r="K142" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L142" s="41"/>
-      <c r="M142" s="41"/>
-      <c r="N142" s="41"/>
-      <c r="O142" s="41"/>
-      <c r="P142" s="42"/>
+      <c r="L142" s="47"/>
+      <c r="M142" s="47"/>
+      <c r="N142" s="47"/>
+      <c r="O142" s="47"/>
+      <c r="P142" s="48"/>
       <c r="X142" s="13"/>
       <c r="Y142" s="13"/>
       <c r="Z142" s="13"/>
       <c r="AA142" s="13"/>
     </row>
     <row r="143" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B143" s="40" t="s">
+      <c r="B143" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C143" s="41"/>
-      <c r="D143" s="41"/>
-      <c r="E143" s="41"/>
-      <c r="F143" s="41"/>
-      <c r="G143" s="42"/>
-      <c r="K143" s="40" t="s">
+      <c r="C143" s="47"/>
+      <c r="D143" s="47"/>
+      <c r="E143" s="47"/>
+      <c r="F143" s="47"/>
+      <c r="G143" s="48"/>
+      <c r="K143" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="L143" s="41"/>
-      <c r="M143" s="41"/>
-      <c r="N143" s="41"/>
-      <c r="O143" s="41"/>
-      <c r="P143" s="42"/>
+      <c r="L143" s="47"/>
+      <c r="M143" s="47"/>
+      <c r="N143" s="47"/>
+      <c r="O143" s="47"/>
+      <c r="P143" s="48"/>
       <c r="X143" s="13"/>
       <c r="Y143" s="13"/>
       <c r="Z143" s="13"/>
       <c r="AA143" s="13"/>
     </row>
     <row r="144" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B144" s="40" t="s">
+      <c r="B144" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C144" s="41"/>
-      <c r="D144" s="41"/>
-      <c r="E144" s="41"/>
-      <c r="F144" s="41"/>
-      <c r="G144" s="42"/>
-      <c r="K144" s="40" t="s">
+      <c r="C144" s="47"/>
+      <c r="D144" s="47"/>
+      <c r="E144" s="47"/>
+      <c r="F144" s="47"/>
+      <c r="G144" s="48"/>
+      <c r="K144" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L144" s="41"/>
-      <c r="M144" s="41"/>
-      <c r="N144" s="41"/>
-      <c r="O144" s="41"/>
-      <c r="P144" s="42"/>
+      <c r="L144" s="47"/>
+      <c r="M144" s="47"/>
+      <c r="N144" s="47"/>
+      <c r="O144" s="47"/>
+      <c r="P144" s="48"/>
       <c r="X144" s="13"/>
       <c r="Y144" s="13"/>
       <c r="Z144" s="13"/>
       <c r="AA144" s="13"/>
     </row>
     <row r="145" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B145" s="40" t="s">
+      <c r="B145" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C145" s="41"/>
-      <c r="D145" s="41"/>
-      <c r="E145" s="41"/>
-      <c r="F145" s="41"/>
-      <c r="G145" s="42"/>
-      <c r="K145" s="40" t="s">
+      <c r="C145" s="47"/>
+      <c r="D145" s="47"/>
+      <c r="E145" s="47"/>
+      <c r="F145" s="47"/>
+      <c r="G145" s="48"/>
+      <c r="K145" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="L145" s="41"/>
-      <c r="M145" s="41"/>
-      <c r="N145" s="41"/>
-      <c r="O145" s="41"/>
-      <c r="P145" s="42"/>
+      <c r="L145" s="47"/>
+      <c r="M145" s="47"/>
+      <c r="N145" s="47"/>
+      <c r="O145" s="47"/>
+      <c r="P145" s="48"/>
       <c r="X145" s="15"/>
       <c r="Y145" s="13"/>
       <c r="Z145" s="13"/>
@@ -3817,6 +3820,189 @@
     </row>
   </sheetData>
   <mergeCells count="207">
+    <mergeCell ref="B112:G112"/>
+    <mergeCell ref="B113:G113"/>
+    <mergeCell ref="B114:G114"/>
+    <mergeCell ref="B115:G115"/>
+    <mergeCell ref="K112:P112"/>
+    <mergeCell ref="K113:P113"/>
+    <mergeCell ref="K114:P114"/>
+    <mergeCell ref="K115:P115"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B104:G104"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B107:G107"/>
+    <mergeCell ref="K103:P103"/>
+    <mergeCell ref="K104:P104"/>
+    <mergeCell ref="K105:P105"/>
+    <mergeCell ref="K107:P107"/>
+    <mergeCell ref="B106:G106"/>
+    <mergeCell ref="K106:P106"/>
+    <mergeCell ref="K79:P79"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="K92:P92"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:G88"/>
+    <mergeCell ref="B89:G89"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B78:G78"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="B80:G80"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="B82:G82"/>
+    <mergeCell ref="K86:P86"/>
+    <mergeCell ref="K78:P78"/>
+    <mergeCell ref="B145:G145"/>
+    <mergeCell ref="B124:G124"/>
+    <mergeCell ref="B125:G125"/>
+    <mergeCell ref="B126:G126"/>
+    <mergeCell ref="B127:G127"/>
+    <mergeCell ref="B128:G128"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B135:G135"/>
+    <mergeCell ref="B136:G136"/>
+    <mergeCell ref="B137:G137"/>
+    <mergeCell ref="B130:G130"/>
+    <mergeCell ref="B133:G133"/>
+    <mergeCell ref="B138:G138"/>
+    <mergeCell ref="B139:G139"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="B141:G141"/>
+    <mergeCell ref="B142:G142"/>
+    <mergeCell ref="B143:G143"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B144:G144"/>
+    <mergeCell ref="B102:G102"/>
+    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="B94:G94"/>
+    <mergeCell ref="B95:G95"/>
+    <mergeCell ref="B96:G96"/>
+    <mergeCell ref="B97:G97"/>
+    <mergeCell ref="B98:G98"/>
+    <mergeCell ref="B101:G101"/>
+    <mergeCell ref="B108:G108"/>
+    <mergeCell ref="B109:G109"/>
+    <mergeCell ref="B91:G91"/>
+    <mergeCell ref="B93:G93"/>
+    <mergeCell ref="B99:G99"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="K145:P145"/>
+    <mergeCell ref="K95:P95"/>
+    <mergeCell ref="K109:P109"/>
+    <mergeCell ref="K118:P118"/>
+    <mergeCell ref="K122:P122"/>
+    <mergeCell ref="K123:P123"/>
+    <mergeCell ref="K137:P137"/>
+    <mergeCell ref="K138:P138"/>
+    <mergeCell ref="K139:P139"/>
+    <mergeCell ref="K144:P144"/>
+    <mergeCell ref="K142:P142"/>
+    <mergeCell ref="K143:P143"/>
+    <mergeCell ref="K141:P141"/>
+    <mergeCell ref="K140:P140"/>
+    <mergeCell ref="K124:P124"/>
+    <mergeCell ref="K99:P99"/>
+    <mergeCell ref="K100:P100"/>
+    <mergeCell ref="K119:P119"/>
+    <mergeCell ref="K102:P102"/>
+    <mergeCell ref="K120:P120"/>
+    <mergeCell ref="K111:P111"/>
+    <mergeCell ref="K130:P130"/>
+    <mergeCell ref="K133:P133"/>
+    <mergeCell ref="K80:P80"/>
+    <mergeCell ref="K81:P81"/>
+    <mergeCell ref="K83:P83"/>
+    <mergeCell ref="K97:P97"/>
+    <mergeCell ref="K110:P110"/>
+    <mergeCell ref="K117:P117"/>
+    <mergeCell ref="K116:P116"/>
+    <mergeCell ref="K108:P108"/>
+    <mergeCell ref="K101:P101"/>
+    <mergeCell ref="K98:P98"/>
+    <mergeCell ref="K87:P87"/>
+    <mergeCell ref="K91:P91"/>
+    <mergeCell ref="K93:P93"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="M69:O69"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="G5:P5"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B48:F48"/>
+    <mergeCell ref="K88:P88"/>
+    <mergeCell ref="K89:P89"/>
+    <mergeCell ref="K90:P90"/>
+    <mergeCell ref="K94:P94"/>
+    <mergeCell ref="K96:P96"/>
+    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="M7:N66"/>
+    <mergeCell ref="K85:P85"/>
+    <mergeCell ref="K82:P82"/>
+    <mergeCell ref="K84:P84"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B84:G84"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="B86:G86"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
     <mergeCell ref="B110:G110"/>
     <mergeCell ref="B116:G116"/>
     <mergeCell ref="B117:G117"/>
@@ -3841,189 +4027,6 @@
     <mergeCell ref="K132:P132"/>
     <mergeCell ref="K129:P129"/>
     <mergeCell ref="K121:P121"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="K88:P88"/>
-    <mergeCell ref="K89:P89"/>
-    <mergeCell ref="K90:P90"/>
-    <mergeCell ref="K94:P94"/>
-    <mergeCell ref="K96:P96"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="M7:N66"/>
-    <mergeCell ref="K85:P85"/>
-    <mergeCell ref="K82:P82"/>
-    <mergeCell ref="K84:P84"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B84:G84"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="B86:G86"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="M69:O69"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="G5:P5"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="K80:P80"/>
-    <mergeCell ref="K81:P81"/>
-    <mergeCell ref="K83:P83"/>
-    <mergeCell ref="K97:P97"/>
-    <mergeCell ref="K110:P110"/>
-    <mergeCell ref="K117:P117"/>
-    <mergeCell ref="K116:P116"/>
-    <mergeCell ref="K108:P108"/>
-    <mergeCell ref="K101:P101"/>
-    <mergeCell ref="K98:P98"/>
-    <mergeCell ref="K87:P87"/>
-    <mergeCell ref="K91:P91"/>
-    <mergeCell ref="K93:P93"/>
-    <mergeCell ref="K145:P145"/>
-    <mergeCell ref="K95:P95"/>
-    <mergeCell ref="K109:P109"/>
-    <mergeCell ref="K118:P118"/>
-    <mergeCell ref="K122:P122"/>
-    <mergeCell ref="K123:P123"/>
-    <mergeCell ref="K137:P137"/>
-    <mergeCell ref="K138:P138"/>
-    <mergeCell ref="K139:P139"/>
-    <mergeCell ref="K144:P144"/>
-    <mergeCell ref="K142:P142"/>
-    <mergeCell ref="K143:P143"/>
-    <mergeCell ref="K141:P141"/>
-    <mergeCell ref="K140:P140"/>
-    <mergeCell ref="K124:P124"/>
-    <mergeCell ref="K99:P99"/>
-    <mergeCell ref="K100:P100"/>
-    <mergeCell ref="K119:P119"/>
-    <mergeCell ref="K102:P102"/>
-    <mergeCell ref="K120:P120"/>
-    <mergeCell ref="K111:P111"/>
-    <mergeCell ref="K130:P130"/>
-    <mergeCell ref="K133:P133"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B144:G144"/>
-    <mergeCell ref="B102:G102"/>
-    <mergeCell ref="B90:G90"/>
-    <mergeCell ref="B94:G94"/>
-    <mergeCell ref="B95:G95"/>
-    <mergeCell ref="B96:G96"/>
-    <mergeCell ref="B97:G97"/>
-    <mergeCell ref="B98:G98"/>
-    <mergeCell ref="B101:G101"/>
-    <mergeCell ref="B108:G108"/>
-    <mergeCell ref="B109:G109"/>
-    <mergeCell ref="B91:G91"/>
-    <mergeCell ref="B93:G93"/>
-    <mergeCell ref="B99:G99"/>
-    <mergeCell ref="B100:G100"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B145:G145"/>
-    <mergeCell ref="B124:G124"/>
-    <mergeCell ref="B125:G125"/>
-    <mergeCell ref="B126:G126"/>
-    <mergeCell ref="B127:G127"/>
-    <mergeCell ref="B128:G128"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="B135:G135"/>
-    <mergeCell ref="B136:G136"/>
-    <mergeCell ref="B137:G137"/>
-    <mergeCell ref="B130:G130"/>
-    <mergeCell ref="B133:G133"/>
-    <mergeCell ref="B138:G138"/>
-    <mergeCell ref="B139:G139"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="B141:G141"/>
-    <mergeCell ref="B142:G142"/>
-    <mergeCell ref="B143:G143"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B92:G92"/>
-    <mergeCell ref="K92:P92"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:G88"/>
-    <mergeCell ref="B89:G89"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B79:G79"/>
-    <mergeCell ref="B80:G80"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B82:G82"/>
-    <mergeCell ref="K86:P86"/>
-    <mergeCell ref="K78:P78"/>
-    <mergeCell ref="B112:G112"/>
-    <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B114:G114"/>
-    <mergeCell ref="B115:G115"/>
-    <mergeCell ref="K112:P112"/>
-    <mergeCell ref="K113:P113"/>
-    <mergeCell ref="K114:P114"/>
-    <mergeCell ref="K115:P115"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B104:G104"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B107:G107"/>
-    <mergeCell ref="K103:P103"/>
-    <mergeCell ref="K104:P104"/>
-    <mergeCell ref="K105:P105"/>
-    <mergeCell ref="K107:P107"/>
-    <mergeCell ref="B106:G106"/>
-    <mergeCell ref="K106:P106"/>
-    <mergeCell ref="K79:P79"/>
   </mergeCells>
   <conditionalFormatting sqref="J36:K36">
     <cfRule type="colorScale" priority="65">
@@ -4169,7 +4172,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15 K15 I15 G15">
+  <conditionalFormatting sqref="K15 O15 I15 G15">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -4217,7 +4220,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O13 K13 I13 G13">
+  <conditionalFormatting sqref="K13 O13 I13 G13">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -4265,7 +4268,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O11 K11 I11 G11">
+  <conditionalFormatting sqref="K11 O11 I11 G11">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -4313,7 +4316,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J21 J23">
+  <conditionalFormatting sqref="J23 J21">
     <cfRule type="colorScale" priority="218">
       <colorScale>
         <cfvo type="min"/>
@@ -4385,7 +4388,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22 I22">
+  <conditionalFormatting sqref="I22 K22">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>